<commit_message>
Removed the outlier ICIs
</commit_message>
<xml_diff>
--- a/SpermWhales/Encounter1_S.xlsx
+++ b/SpermWhales/Encounter1_S.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
   <si>
     <t>tbin</t>
   </si>
@@ -45,7 +45,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -76,17 +76,21 @@
     </border>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true" applyBorder="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true" applyBorder="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,16 +385,16 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1"/>
     </row>
     <row r="2">
-      <c r="A2" s="5">
+      <c r="A2" s="7">
         <v>43585.840715850121</v>
       </c>
       <c r="B2">
@@ -398,7 +402,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5">
+      <c r="A3" s="7">
         <v>43585.840731020318</v>
       </c>
       <c r="B3">
@@ -406,7 +410,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5">
+      <c r="A4" s="7">
         <v>43585.841044469038</v>
       </c>
       <c r="B4">
@@ -414,7 +418,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5">
+      <c r="A5" s="7">
         <v>43585.841058316524</v>
       </c>
       <c r="B5">
@@ -422,7 +426,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="5">
+      <c r="A6" s="7">
         <v>43585.841071297305</v>
       </c>
       <c r="B6">
@@ -430,7 +434,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5">
+      <c r="A7" s="7">
         <v>43585.841081745457</v>
       </c>
       <c r="B7">
@@ -438,7 +442,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="5">
+      <c r="A8" s="7">
         <v>43585.841090766597</v>
       </c>
       <c r="B8">
@@ -446,7 +450,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="5">
+      <c r="A9" s="7">
         <v>43585.841099718586</v>
       </c>
       <c r="B9">
@@ -454,7 +458,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="5">
+      <c r="A10" s="7">
         <v>43585.841401556732</v>
       </c>
       <c r="B10">
@@ -462,7 +466,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="5">
+      <c r="A11" s="7">
         <v>43585.841415913193</v>
       </c>
       <c r="B11">
@@ -470,7 +474,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="5">
+      <c r="A12" s="7">
         <v>43585.841690794681</v>
       </c>
       <c r="B12">
@@ -478,7 +482,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="5">
+      <c r="A13" s="7">
         <v>43585.841704762657</v>
       </c>
       <c r="B13">
@@ -486,7 +490,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="5">
+      <c r="A14" s="7">
         <v>43585.841719100492</v>
       </c>
       <c r="B14">
@@ -494,7 +498,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="5">
+      <c r="A15" s="7">
         <v>43585.841733220499</v>
       </c>
       <c r="B15">
@@ -502,7 +506,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="5">
+      <c r="A16" s="7">
         <v>43585.841748178827</v>
       </c>
       <c r="B16">
@@ -510,7 +514,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="5">
+      <c r="A17" s="7">
         <v>43585.841763657518</v>
       </c>
       <c r="B17">
@@ -518,7 +522,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="5">
+      <c r="A18" s="7">
         <v>43585.841778987669</v>
       </c>
       <c r="B18">
@@ -526,7 +530,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="5">
+      <c r="A19" s="7">
         <v>43585.841787181213</v>
       </c>
       <c r="B19">
@@ -534,7 +538,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="5">
+      <c r="A20" s="7">
         <v>43585.841794488369</v>
       </c>
       <c r="B20">
@@ -542,7 +546,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="5">
+      <c r="A21" s="7">
         <v>43585.841797969886</v>
       </c>
       <c r="B21">
@@ -550,7 +554,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="5">
+      <c r="A22" s="7">
         <v>43585.841809722711</v>
       </c>
       <c r="B22">
@@ -558,7 +562,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="5">
+      <c r="A23" s="7">
         <v>43585.841821674025</v>
       </c>
       <c r="B23">
@@ -566,7 +570,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="5">
+      <c r="A24" s="7">
         <v>43585.841871691286</v>
       </c>
       <c r="B24">
@@ -574,7 +578,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="5">
+      <c r="A25" s="7">
         <v>43585.841884244117</v>
       </c>
       <c r="B25">
@@ -582,7 +586,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="5">
+      <c r="A26" s="7">
         <v>43585.841896645725</v>
       </c>
       <c r="B26">
@@ -590,7 +594,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="5">
+      <c r="A27" s="7">
         <v>43585.842064975062</v>
       </c>
       <c r="B27">
@@ -598,7 +602,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="5">
+      <c r="A28" s="7">
         <v>43585.842077846406</v>
       </c>
       <c r="B28">
@@ -606,7 +610,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="5">
+      <c r="A29" s="7">
         <v>43585.842088334728</v>
       </c>
       <c r="B29">
@@ -614,7 +618,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="5">
+      <c r="A30" s="7">
         <v>43585.842300204211</v>
       </c>
       <c r="B30">
@@ -622,7 +626,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="5">
+      <c r="A31" s="7">
         <v>43585.842349397019</v>
       </c>
       <c r="B31">
@@ -630,7 +634,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="5">
+      <c r="A32" s="7">
         <v>43585.84236596548</v>
       </c>
       <c r="B32">
@@ -638,7 +642,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="5">
+      <c r="A33" s="7">
         <v>43585.842431212659</v>
       </c>
       <c r="B33">
@@ -646,7 +650,7 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="5">
+      <c r="A34" s="7">
         <v>43585.842448086478</v>
       </c>
       <c r="B34">
@@ -654,7 +658,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="5">
+      <c r="A35" s="7">
         <v>43585.842464990332</v>
       </c>
       <c r="B35">
@@ -662,7 +666,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="5">
+      <c r="A36" s="7">
         <v>43585.842481952277</v>
       </c>
       <c r="B36">
@@ -670,7 +674,7 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="5">
+      <c r="A37" s="7">
         <v>43585.842499040999</v>
       </c>
       <c r="B37">
@@ -678,7 +682,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="5">
+      <c r="A38" s="7">
         <v>43585.84251601249</v>
       </c>
       <c r="B38">
@@ -686,7 +690,7 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="5">
+      <c r="A39" s="7">
         <v>43585.842532096656</v>
       </c>
       <c r="B39">
@@ -694,7 +698,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="5">
+      <c r="A40" s="7">
         <v>43585.842576938332</v>
       </c>
       <c r="B40">
@@ -702,7 +706,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="5">
+      <c r="A41" s="7">
         <v>43585.842581706005</v>
       </c>
       <c r="B41">
@@ -710,7 +714,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="5">
+      <c r="A42" s="7">
         <v>43585.842598725692</v>
       </c>
       <c r="B42">
@@ -718,7 +722,7 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="5">
+      <c r="A43" s="7">
         <v>43585.842751239776</v>
       </c>
       <c r="B43">
@@ -726,7 +730,7 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="5">
+      <c r="A44" s="7">
         <v>43585.842804556247</v>
       </c>
       <c r="B44">
@@ -734,7 +738,7 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="5">
+      <c r="A45" s="7">
         <v>43585.842815635959</v>
       </c>
       <c r="B45">
@@ -742,7 +746,7 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="5">
+      <c r="A46" s="7">
         <v>43585.842826162116</v>
       </c>
       <c r="B46">
@@ -750,7 +754,7 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="5">
+      <c r="A47" s="7">
         <v>43585.842838044395</v>
       </c>
       <c r="B47">
@@ -758,7 +762,7 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="5">
+      <c r="A48" s="7">
         <v>43585.842860309873</v>
       </c>
       <c r="B48">
@@ -766,7 +770,7 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="5">
+      <c r="A49" s="7">
         <v>43585.842872129404</v>
       </c>
       <c r="B49">
@@ -774,7 +778,7 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="5">
+      <c r="A50" s="7">
         <v>43585.842883898062</v>
       </c>
       <c r="B50">
@@ -782,7 +786,7 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="5">
+      <c r="A51" s="7">
         <v>43585.84310239146</v>
       </c>
       <c r="B51">
@@ -790,7 +794,7 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="5">
+      <c r="A52" s="7">
         <v>43585.843225193326</v>
       </c>
       <c r="B52">
@@ -798,7 +802,7 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="5">
+      <c r="A53" s="7">
         <v>43585.843237082823</v>
       </c>
       <c r="B53">
@@ -806,7 +810,7 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="5">
+      <c r="A54" s="7">
         <v>43585.843307295116</v>
       </c>
       <c r="B54">
@@ -814,7 +818,7 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="5">
+      <c r="A55" s="7">
         <v>43585.843311355682</v>
       </c>
       <c r="B55">
@@ -822,7 +826,7 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="5">
+      <c r="A56" s="7">
         <v>43585.843319456792</v>
       </c>
       <c r="B56">
@@ -830,7 +834,7 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="5">
+      <c r="A57" s="7">
         <v>43585.843331799369</v>
       </c>
       <c r="B57">
@@ -838,7 +842,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="5">
+      <c r="A58" s="7">
         <v>43585.843344341258</v>
       </c>
       <c r="B58">
@@ -846,7 +850,7 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="5">
+      <c r="A59" s="7">
         <v>43585.84335740516</v>
       </c>
       <c r="B59">
@@ -854,7 +858,7 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="5">
+      <c r="A60" s="7">
         <v>43585.843370794668</v>
       </c>
       <c r="B60">
@@ -862,7 +866,7 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="5">
+      <c r="A61" s="7">
         <v>43585.843383210828</v>
       </c>
       <c r="B61">
@@ -870,7 +874,7 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="5">
+      <c r="A62" s="7">
         <v>43585.843394905212</v>
       </c>
       <c r="B62">
@@ -878,7 +882,7 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="5">
+      <c r="A63" s="7">
         <v>43585.843399847858</v>
       </c>
       <c r="B63">
@@ -886,7 +890,7 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="5">
+      <c r="A64" s="7">
         <v>43585.843414838891</v>
       </c>
       <c r="B64">
@@ -894,7 +898,7 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="5">
+      <c r="A65" s="7">
         <v>43585.843429452507</v>
       </c>
       <c r="B65">
@@ -902,7 +906,7 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="5">
+      <c r="A66" s="7">
         <v>43585.843443304999</v>
       </c>
       <c r="B66">
@@ -910,7 +914,7 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="5">
+      <c r="A67" s="7">
         <v>43585.843454776106</v>
       </c>
       <c r="B67">
@@ -918,7 +922,7 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="5">
+      <c r="A68" s="7">
         <v>43585.843459588476</v>
       </c>
       <c r="B68">
@@ -926,7 +930,7 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="5">
+      <c r="A69" s="7">
         <v>43585.843465970829</v>
       </c>
       <c r="B69">
@@ -934,7 +938,7 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="5">
+      <c r="A70" s="7">
         <v>43585.843644010485</v>
       </c>
       <c r="B70">
@@ -942,7 +946,7 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="5">
+      <c r="A71" s="7">
         <v>43585.843648022157</v>
       </c>
       <c r="B71">
@@ -950,7 +954,7 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="5">
+      <c r="A72" s="7">
         <v>43585.843655379023</v>
       </c>
       <c r="B72">
@@ -958,7 +962,7 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="5">
+      <c r="A73" s="7">
         <v>43585.843667704263</v>
       </c>
       <c r="B73">
@@ -966,7 +970,7 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="5">
+      <c r="A74" s="7">
         <v>43585.843682644772</v>
       </c>
       <c r="B74">
@@ -974,7 +978,7 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="5">
+      <c r="A75" s="7">
         <v>43585.843734285445</v>
       </c>
       <c r="B75">
@@ -982,7 +986,7 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="5">
+      <c r="A76" s="7">
         <v>43585.843752585119</v>
       </c>
       <c r="B76">
@@ -990,7 +994,7 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="5">
+      <c r="A77" s="7">
         <v>43585.843770156614</v>
       </c>
       <c r="B77">
@@ -998,7 +1002,7 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="5">
+      <c r="A78" s="7">
         <v>43585.843787767226</v>
       </c>
       <c r="B78">
@@ -1006,7 +1010,7 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="5">
+      <c r="A79" s="7">
         <v>43585.843806418939</v>
       </c>
       <c r="B79">
@@ -1014,7 +1018,7 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="5">
+      <c r="A80" s="7">
         <v>43585.843823781244</v>
       </c>
       <c r="B80">
@@ -1022,7 +1026,7 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="5">
+      <c r="A81" s="7">
         <v>43585.843841164016</v>
       </c>
       <c r="B81">
@@ -1030,7 +1034,7 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="5">
+      <c r="A82" s="7">
         <v>43585.84385431488</v>
       </c>
       <c r="B82">
@@ -1038,7 +1042,7 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="5">
+      <c r="A83" s="7">
         <v>43585.843859678018</v>
       </c>
       <c r="B83">
@@ -1046,7 +1050,7 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="5">
+      <c r="A84" s="7">
         <v>43585.843866237672</v>
       </c>
       <c r="B84">
@@ -1054,7 +1058,7 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="5">
+      <c r="A85" s="7">
         <v>43585.843877182218</v>
       </c>
       <c r="B85">
@@ -1062,7 +1066,7 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="5">
+      <c r="A86" s="7">
         <v>43585.843890062999</v>
       </c>
       <c r="B86">
@@ -1070,7 +1074,7 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="5">
+      <c r="A87" s="7">
         <v>43585.843902152381</v>
       </c>
       <c r="B87">
@@ -1078,7 +1082,7 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="5">
+      <c r="A88" s="7">
         <v>43585.843914337689</v>
       </c>
       <c r="B88">
@@ -1086,7 +1090,7 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="5">
+      <c r="A89" s="7">
         <v>43585.843926208559</v>
       </c>
       <c r="B89">
@@ -1094,7 +1098,7 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="5">
+      <c r="A90" s="7">
         <v>43585.843938436825</v>
       </c>
       <c r="B90">
@@ -1102,7 +1106,7 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="5">
+      <c r="A91" s="7">
         <v>43585.843949652626</v>
       </c>
       <c r="B91">
@@ -1110,7 +1114,7 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="5">
+      <c r="A92" s="7">
         <v>43585.843960768427</v>
       </c>
       <c r="B92">
@@ -1118,7 +1122,7 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="5">
+      <c r="A93" s="7">
         <v>43585.843972330556</v>
       </c>
       <c r="B93">
@@ -1126,7 +1130,7 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="5">
+      <c r="A94" s="7">
         <v>43585.84398458444</v>
       </c>
       <c r="B94">
@@ -1134,7 +1138,7 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="5">
+      <c r="A95" s="7">
         <v>43585.843996373238</v>
       </c>
       <c r="B95">
@@ -1142,7 +1146,7 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="5">
+      <c r="A96" s="7">
         <v>43585.844008783461</v>
       </c>
       <c r="B96">
@@ -1150,7 +1154,7 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="5">
+      <c r="A97" s="7">
         <v>43585.844021560275</v>
       </c>
       <c r="B97">
@@ -1158,7 +1162,7 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="5">
+      <c r="A98" s="7">
         <v>43585.844034064095</v>
       </c>
       <c r="B98">
@@ -1166,7 +1170,7 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="5">
+      <c r="A99" s="7">
         <v>43585.844046085374</v>
       </c>
       <c r="B99">
@@ -1174,7 +1178,7 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="5">
+      <c r="A100" s="7">
         <v>43585.844058027025</v>
       </c>
       <c r="B100">
@@ -1182,7 +1186,7 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="5">
+      <c r="A101" s="7">
         <v>43585.844070344574</v>
       </c>
       <c r="B101">
@@ -1190,7 +1194,7 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="5">
+      <c r="A102" s="7">
         <v>43585.844082950265</v>
       </c>
       <c r="B102">
@@ -1198,7 +1202,7 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="5">
+      <c r="A103" s="7">
         <v>43585.844095223234</v>
       </c>
       <c r="B103">
@@ -1206,7 +1210,7 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="5">
+      <c r="A104" s="7">
         <v>43585.844107813318</v>
       </c>
       <c r="B104">
@@ -1214,7 +1218,7 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="5">
+      <c r="A105" s="7">
         <v>43585.844768323463</v>
       </c>
       <c r="B105">
@@ -1222,7 +1226,7 @@
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="5">
+      <c r="A106" s="7">
         <v>43585.844776571728</v>
       </c>
       <c r="B106">
@@ -1230,7 +1234,7 @@
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="5">
+      <c r="A107" s="7">
         <v>43585.844785296242</v>
       </c>
       <c r="B107">
@@ -1238,7 +1242,7 @@
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="5">
+      <c r="A108" s="7">
         <v>43585.844794197241</v>
       </c>
       <c r="B108">
@@ -1246,7 +1250,7 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="5">
+      <c r="A109" s="7">
         <v>43585.844803359942</v>
       </c>
       <c r="B109">
@@ -1254,7 +1258,7 @@
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="5">
+      <c r="A110" s="7">
         <v>43585.84482180397</v>
       </c>
       <c r="B110">
@@ -1262,7 +1266,7 @@
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="5">
+      <c r="A111" s="7">
         <v>43585.844828433241</v>
       </c>
       <c r="B111">
@@ -1270,7 +1274,7 @@
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="5">
+      <c r="A112" s="7">
         <v>43585.844850008842</v>
       </c>
       <c r="B112">
@@ -1278,7 +1282,7 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="5">
+      <c r="A113" s="7">
         <v>43585.8449107419</v>
       </c>
       <c r="B113">
@@ -1286,7 +1290,7 @@
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="5">
+      <c r="A114" s="7">
         <v>43585.844918646733</v>
       </c>
       <c r="B114">
@@ -1294,7 +1298,7 @@
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="5">
+      <c r="A115" s="7">
         <v>43585.84492785122</v>
       </c>
       <c r="B115">
@@ -1302,7 +1306,7 @@
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="5">
+      <c r="A116" s="7">
         <v>43585.845026769792</v>
       </c>
       <c r="B116">
@@ -1310,7 +1314,7 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="5">
+      <c r="A117" s="7">
         <v>43585.845034999424</v>
       </c>
       <c r="B117">
@@ -1318,7 +1322,7 @@
       </c>
     </row>
     <row r="118">
-      <c r="A118" s="5">
+      <c r="A118" s="7">
         <v>43585.845044281101</v>
       </c>
       <c r="B118">
@@ -1326,7 +1330,7 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="5">
+      <c r="A119" s="7">
         <v>43585.845063277055</v>
       </c>
       <c r="B119">
@@ -1334,7 +1338,7 @@
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="5">
+      <c r="A120" s="7">
         <v>43585.845556687796</v>
       </c>
       <c r="B120">
@@ -1342,7 +1346,7 @@
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="5">
+      <c r="A121" s="7">
         <v>43585.846288154251</v>
       </c>
       <c r="B121">
@@ -1350,7 +1354,7 @@
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="5">
+      <c r="A122" s="7">
         <v>43585.846295420779</v>
       </c>
       <c r="B122">
@@ -1358,7 +1362,7 @@
       </c>
     </row>
     <row r="123">
-      <c r="A123" s="5">
+      <c r="A123" s="7">
         <v>43585.846302805468</v>
       </c>
       <c r="B123">
@@ -1366,7 +1370,7 @@
       </c>
     </row>
     <row r="124">
-      <c r="A124" s="5">
+      <c r="A124" s="7">
         <v>43585.846310260007</v>
       </c>
       <c r="B124">
@@ -1374,7 +1378,7 @@
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="5">
+      <c r="A125" s="7">
         <v>43585.846317797434</v>
       </c>
       <c r="B125">
@@ -1382,7 +1386,7 @@
       </c>
     </row>
     <row r="126">
-      <c r="A126" s="5">
+      <c r="A126" s="7">
         <v>43585.846325494924</v>
       </c>
       <c r="B126">
@@ -1390,7 +1394,7 @@
       </c>
     </row>
     <row r="127">
-      <c r="A127" s="5">
+      <c r="A127" s="7">
         <v>43585.846333371941</v>
       </c>
       <c r="B127">
@@ -1398,7 +1402,7 @@
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="5">
+      <c r="A128" s="7">
         <v>43585.846341370729</v>
       </c>
       <c r="B128">
@@ -1406,7 +1410,7 @@
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="5">
+      <c r="A129" s="7">
         <v>43585.846349443309</v>
       </c>
       <c r="B129">
@@ -1414,7 +1418,7 @@
       </c>
     </row>
     <row r="130">
-      <c r="A130" s="5">
+      <c r="A130" s="7">
         <v>43585.846451296704</v>
       </c>
       <c r="B130">
@@ -1422,7 +1426,7 @@
       </c>
     </row>
     <row r="131">
-      <c r="A131" s="5">
+      <c r="A131" s="7">
         <v>43585.8464700568</v>
       </c>
       <c r="B131">
@@ -1430,7 +1434,7 @@
       </c>
     </row>
     <row r="132">
-      <c r="A132" s="5">
+      <c r="A132" s="7">
         <v>43585.846477589337</v>
       </c>
       <c r="B132">
@@ -1438,7 +1442,7 @@
       </c>
     </row>
     <row r="133">
-      <c r="A133" s="5">
+      <c r="A133" s="7">
         <v>43585.846485753777</v>
       </c>
       <c r="B133">
@@ -1446,7 +1450,7 @@
       </c>
     </row>
     <row r="134">
-      <c r="A134" s="5">
+      <c r="A134" s="7">
         <v>43585.846834442928</v>
       </c>
       <c r="B134">
@@ -1454,7 +1458,7 @@
       </c>
     </row>
     <row r="135">
-      <c r="A135" s="5">
+      <c r="A135" s="7">
         <v>43585.846846495755</v>
       </c>
       <c r="B135">
@@ -1462,7 +1466,7 @@
       </c>
     </row>
     <row r="136">
-      <c r="A136" s="5">
+      <c r="A136" s="7">
         <v>43585.846853023511</v>
       </c>
       <c r="B136">
@@ -1470,7 +1474,7 @@
       </c>
     </row>
     <row r="137">
-      <c r="A137" s="5">
+      <c r="A137" s="7">
         <v>43585.847075873753</v>
       </c>
       <c r="B137">
@@ -1478,7 +1482,7 @@
       </c>
     </row>
     <row r="138">
-      <c r="A138" s="5">
+      <c r="A138" s="7">
         <v>43585.847099012346</v>
       </c>
       <c r="B138">
@@ -1486,7 +1490,7 @@
       </c>
     </row>
     <row r="139">
-      <c r="A139" s="5">
+      <c r="A139" s="7">
         <v>43585.847257048357</v>
       </c>
       <c r="B139">
@@ -1494,7 +1498,7 @@
       </c>
     </row>
     <row r="140">
-      <c r="A140" s="5">
+      <c r="A140" s="7">
         <v>43585.847270789091</v>
       </c>
       <c r="B140">
@@ -1502,7 +1506,7 @@
       </c>
     </row>
     <row r="141">
-      <c r="A141" s="5">
+      <c r="A141" s="7">
         <v>43585.84728419804</v>
       </c>
       <c r="B141">
@@ -1510,7 +1514,7 @@
       </c>
     </row>
     <row r="142">
-      <c r="A142" s="5">
+      <c r="A142" s="7">
         <v>43585.847777782947</v>
       </c>
       <c r="B142">
@@ -1518,7 +1522,7 @@
       </c>
     </row>
     <row r="143">
-      <c r="A143" s="5">
+      <c r="A143" s="7">
         <v>43585.847898194683</v>
       </c>
       <c r="B143">
@@ -1526,7 +1530,7 @@
       </c>
     </row>
     <row r="144">
-      <c r="A144" s="5">
+      <c r="A144" s="7">
         <v>43585.847905522212</v>
       </c>
       <c r="B144">
@@ -1534,7 +1538,7 @@
       </c>
     </row>
     <row r="145">
-      <c r="A145" s="5">
+      <c r="A145" s="7">
         <v>43585.847912758589</v>
       </c>
       <c r="B145">
@@ -1542,7 +1546,7 @@
       </c>
     </row>
     <row r="146">
-      <c r="A146" s="5">
+      <c r="A146" s="7">
         <v>43585.847920786007</v>
       </c>
       <c r="B146">
@@ -1550,7 +1554,7 @@
       </c>
     </row>
     <row r="147">
-      <c r="A147" s="5">
+      <c r="A147" s="7">
         <v>43585.84792728466</v>
       </c>
       <c r="B147">
@@ -1558,7 +1562,7 @@
       </c>
     </row>
     <row r="148">
-      <c r="A148" s="5">
+      <c r="A148" s="7">
         <v>43585.847934502177</v>
       </c>
       <c r="B148">
@@ -1566,7 +1570,7 @@
       </c>
     </row>
     <row r="149">
-      <c r="A149" s="5">
+      <c r="A149" s="7">
         <v>43585.847942243214</v>
       </c>
       <c r="B149">
@@ -1574,7 +1578,7 @@
       </c>
     </row>
     <row r="150">
-      <c r="A150" s="5">
+      <c r="A150" s="7">
         <v>43585.84795068251</v>
       </c>
       <c r="B150">
@@ -1582,7 +1586,7 @@
       </c>
     </row>
     <row r="151">
-      <c r="A151" s="5">
+      <c r="A151" s="7">
         <v>43585.848075106507</v>
       </c>
       <c r="B151">
@@ -1590,7 +1594,7 @@
       </c>
     </row>
     <row r="152">
-      <c r="A152" s="5">
+      <c r="A152" s="7">
         <v>43585.848690364161</v>
       </c>
       <c r="B152">
@@ -1598,7 +1602,7 @@
       </c>
     </row>
     <row r="153">
-      <c r="A153" s="5">
+      <c r="A153" s="7">
         <v>43585.848701021641</v>
       </c>
       <c r="B153">
@@ -1606,7 +1610,7 @@
       </c>
     </row>
     <row r="154">
-      <c r="A154" s="5">
+      <c r="A154" s="7">
         <v>43585.848712101928</v>
       </c>
       <c r="B154">
@@ -1614,7 +1618,7 @@
       </c>
     </row>
     <row r="155">
-      <c r="A155" s="5">
+      <c r="A155" s="7">
         <v>43585.848723550444</v>
       </c>
       <c r="B155">
@@ -1622,7 +1626,7 @@
       </c>
     </row>
     <row r="156">
-      <c r="A156" s="5">
+      <c r="A156" s="7">
         <v>43585.849062200286</v>
       </c>
       <c r="B156">
@@ -1630,7 +1634,7 @@
       </c>
     </row>
     <row r="157">
-      <c r="A157" s="5">
+      <c r="A157" s="7">
         <v>43585.84978678741</v>
       </c>
       <c r="B157">
@@ -1638,7 +1642,7 @@
       </c>
     </row>
     <row r="158">
-      <c r="A158" s="5">
+      <c r="A158" s="7">
         <v>43585.849861848052</v>
       </c>
       <c r="B158">
@@ -1646,7 +1650,7 @@
       </c>
     </row>
     <row r="159">
-      <c r="A159" s="5">
+      <c r="A159" s="7">
         <v>43585.849876207998</v>
       </c>
       <c r="B159">
@@ -1654,7 +1658,7 @@
       </c>
     </row>
     <row r="160">
-      <c r="A160" s="5">
+      <c r="A160" s="7">
         <v>43585.84988322563</v>
       </c>
       <c r="B160">
@@ -1662,7 +1666,7 @@
       </c>
     </row>
     <row r="161">
-      <c r="A161" s="5">
+      <c r="A161" s="7">
         <v>43585.849890468875</v>
       </c>
       <c r="B161">
@@ -1670,7 +1674,7 @@
       </c>
     </row>
     <row r="162">
-      <c r="A162" s="5">
+      <c r="A162" s="7">
         <v>43585.849905646872</v>
       </c>
       <c r="B162">
@@ -1678,7 +1682,7 @@
       </c>
     </row>
     <row r="163">
-      <c r="A163" s="5">
+      <c r="A163" s="7">
         <v>43585.84996883804</v>
       </c>
       <c r="B163">
@@ -1686,7 +1690,7 @@
       </c>
     </row>
     <row r="164">
-      <c r="A164" s="5">
+      <c r="A164" s="7">
         <v>43585.850014405325</v>
       </c>
       <c r="B164">
@@ -1694,7 +1698,7 @@
       </c>
     </row>
     <row r="165">
-      <c r="A165" s="5">
+      <c r="A165" s="7">
         <v>43585.850075060036</v>
       </c>
       <c r="B165">
@@ -1702,7 +1706,7 @@
       </c>
     </row>
     <row r="166">
-      <c r="A166" s="5">
+      <c r="A166" s="7">
         <v>43585.850082770456</v>
       </c>
       <c r="B166">
@@ -1710,7 +1714,7 @@
       </c>
     </row>
     <row r="167">
-      <c r="A167" s="5">
+      <c r="A167" s="7">
         <v>43585.850090551547</v>
       </c>
       <c r="B167">
@@ -1718,7 +1722,7 @@
       </c>
     </row>
     <row r="168">
-      <c r="A168" s="5">
+      <c r="A168" s="7">
         <v>43585.85009826639</v>
       </c>
       <c r="B168">
@@ -1726,7 +1730,7 @@
       </c>
     </row>
     <row r="169">
-      <c r="A169" s="5">
+      <c r="A169" s="7">
         <v>43585.850106078433</v>
       </c>
       <c r="B169">
@@ -1734,7 +1738,7 @@
       </c>
     </row>
     <row r="170">
-      <c r="A170" s="5">
+      <c r="A170" s="7">
         <v>43585.850113878725</v>
       </c>
       <c r="B170">
@@ -1742,7 +1746,7 @@
       </c>
     </row>
     <row r="171">
-      <c r="A171" s="5">
+      <c r="A171" s="7">
         <v>43585.850153105333</v>
       </c>
       <c r="B171">
@@ -1750,7 +1754,7 @@
       </c>
     </row>
     <row r="172">
-      <c r="A172" s="5">
+      <c r="A172" s="7">
         <v>43585.850161108421</v>
       </c>
       <c r="B172">
@@ -1758,7 +1762,7 @@
       </c>
     </row>
     <row r="173">
-      <c r="A173" s="5">
+      <c r="A173" s="7">
         <v>43585.850169139332</v>
       </c>
       <c r="B173">
@@ -1766,7 +1770,7 @@
       </c>
     </row>
     <row r="174">
-      <c r="A174" s="5">
+      <c r="A174" s="7">
         <v>43585.850177181535</v>
       </c>
       <c r="B174">
@@ -1774,7 +1778,7 @@
       </c>
     </row>
     <row r="175">
-      <c r="A175" s="5">
+      <c r="A175" s="7">
         <v>43585.850185401388</v>
       </c>
       <c r="B175">
@@ -1782,7 +1786,7 @@
       </c>
     </row>
     <row r="176">
-      <c r="A176" s="5">
+      <c r="A176" s="7">
         <v>43585.85020210372</v>
       </c>
       <c r="B176">
@@ -1790,7 +1794,7 @@
       </c>
     </row>
     <row r="177">
-      <c r="A177" s="5">
+      <c r="A177" s="7">
         <v>43585.850210714038</v>
       </c>
       <c r="B177">
@@ -1798,7 +1802,7 @@
       </c>
     </row>
     <row r="178">
-      <c r="A178" s="5">
+      <c r="A178" s="7">
         <v>43585.85021925671</v>
       </c>
       <c r="B178">
@@ -1806,7 +1810,7 @@
       </c>
     </row>
     <row r="179">
-      <c r="A179" s="5">
+      <c r="A179" s="7">
         <v>43585.850225116708</v>
       </c>
       <c r="B179">
@@ -1814,7 +1818,7 @@
       </c>
     </row>
     <row r="180">
-      <c r="A180" s="5">
+      <c r="A180" s="7">
         <v>43585.850234824349</v>
       </c>
       <c r="B180">
@@ -1822,7 +1826,7 @@
       </c>
     </row>
     <row r="181">
-      <c r="A181" s="5">
+      <c r="A181" s="7">
         <v>43585.850241898792</v>
       </c>
       <c r="B181">
@@ -1830,7 +1834,7 @@
       </c>
     </row>
     <row r="182">
-      <c r="A182" s="5">
+      <c r="A182" s="7">
         <v>43585.850464220974</v>
       </c>
       <c r="B182">
@@ -1838,7 +1842,7 @@
       </c>
     </row>
     <row r="183">
-      <c r="A183" s="5">
+      <c r="A183" s="7">
         <v>43585.850918983226</v>
       </c>
       <c r="B183">
@@ -1846,7 +1850,7 @@
       </c>
     </row>
     <row r="184">
-      <c r="A184" s="5">
+      <c r="A184" s="7">
         <v>43585.850930474116</v>
       </c>
       <c r="B184">
@@ -1854,7 +1858,7 @@
       </c>
     </row>
     <row r="185">
-      <c r="A185" s="5">
+      <c r="A185" s="7">
         <v>43585.850941837765</v>
       </c>
       <c r="B185">
@@ -1862,7 +1866,7 @@
       </c>
     </row>
     <row r="186">
-      <c r="A186" s="5">
+      <c r="A186" s="7">
         <v>43585.851058175671</v>
       </c>
       <c r="B186">
@@ -1870,7 +1874,7 @@
       </c>
     </row>
     <row r="187">
-      <c r="A187" s="5">
+      <c r="A187" s="7">
         <v>43585.851200236706</v>
       </c>
       <c r="B187">
@@ -1878,7 +1882,7 @@
       </c>
     </row>
     <row r="188">
-      <c r="A188" s="5">
+      <c r="A188" s="7">
         <v>43585.851530091022</v>
       </c>
       <c r="B188">
@@ -1886,7 +1890,7 @@
       </c>
     </row>
     <row r="189">
-      <c r="A189" s="5">
+      <c r="A189" s="7">
         <v>43585.851540779811</v>
       </c>
       <c r="B189">
@@ -1894,7 +1898,7 @@
       </c>
     </row>
     <row r="190">
-      <c r="A190" s="5">
+      <c r="A190" s="7">
         <v>43585.85155267315</v>
       </c>
       <c r="B190">
@@ -1902,7 +1906,7 @@
       </c>
     </row>
     <row r="191">
-      <c r="A191" s="5">
+      <c r="A191" s="7">
         <v>43585.851596922381</v>
       </c>
       <c r="B191">
@@ -1910,7 +1914,7 @@
       </c>
     </row>
     <row r="192">
-      <c r="A192" s="5">
+      <c r="A192" s="7">
         <v>43585.851672356366</v>
       </c>
       <c r="B192">
@@ -1918,7 +1922,7 @@
       </c>
     </row>
     <row r="193">
-      <c r="A193" s="5">
+      <c r="A193" s="7">
         <v>43585.851680005086</v>
       </c>
       <c r="B193">
@@ -1926,7 +1930,7 @@
       </c>
     </row>
     <row r="194">
-      <c r="A194" s="5">
+      <c r="A194" s="7">
         <v>43585.851687957533</v>
       </c>
       <c r="B194">
@@ -1934,7 +1938,7 @@
       </c>
     </row>
     <row r="195">
-      <c r="A195" s="5">
+      <c r="A195" s="7">
         <v>43585.851696234546</v>
       </c>
       <c r="B195">
@@ -1942,7 +1946,7 @@
       </c>
     </row>
     <row r="196">
-      <c r="A196" s="5">
+      <c r="A196" s="7">
         <v>43585.851704480592</v>
       </c>
       <c r="B196">
@@ -1950,7 +1954,7 @@
       </c>
     </row>
     <row r="197">
-      <c r="A197" s="5">
+      <c r="A197" s="7">
         <v>43585.851737773861</v>
       </c>
       <c r="B197">
@@ -1958,7 +1962,7 @@
       </c>
     </row>
     <row r="198">
-      <c r="A198" s="5">
+      <c r="A198" s="7">
         <v>43585.851745988475</v>
       </c>
       <c r="B198">
@@ -1966,7 +1970,7 @@
       </c>
     </row>
     <row r="199">
-      <c r="A199" s="5">
+      <c r="A199" s="7">
         <v>43585.851754270494</v>
       </c>
       <c r="B199">
@@ -1974,7 +1978,7 @@
       </c>
     </row>
     <row r="200">
-      <c r="A200" s="5">
+      <c r="A200" s="7">
         <v>43585.852542103268</v>
       </c>
       <c r="B200">
@@ -1982,7 +1986,7 @@
       </c>
     </row>
     <row r="201">
-      <c r="A201" s="5">
+      <c r="A201" s="7">
         <v>43585.852551665273</v>
       </c>
       <c r="B201">
@@ -1990,7 +1994,7 @@
       </c>
     </row>
     <row r="202">
-      <c r="A202" s="5">
+      <c r="A202" s="7">
         <v>43585.852604087668</v>
       </c>
       <c r="B202">
@@ -1998,7 +2002,7 @@
       </c>
     </row>
     <row r="203">
-      <c r="A203" s="5">
+      <c r="A203" s="7">
         <v>43585.852613567375</v>
       </c>
       <c r="B203">
@@ -2006,7 +2010,7 @@
       </c>
     </row>
     <row r="204">
-      <c r="A204" s="5">
+      <c r="A204" s="7">
         <v>43585.852621927042</v>
       </c>
       <c r="B204">
@@ -2014,7 +2018,7 @@
       </c>
     </row>
     <row r="205">
-      <c r="A205" s="5">
+      <c r="A205" s="7">
         <v>43585.852629832458</v>
       </c>
       <c r="B205">
@@ -2022,7 +2026,7 @@
       </c>
     </row>
     <row r="206">
-      <c r="A206" s="5">
+      <c r="A206" s="7">
         <v>43585.852637898875</v>
       </c>
       <c r="B206">
@@ -2030,7 +2034,7 @@
       </c>
     </row>
     <row r="207">
-      <c r="A207" s="5">
+      <c r="A207" s="7">
         <v>43585.852648839355</v>
       </c>
       <c r="B207">
@@ -2038,7 +2042,7 @@
       </c>
     </row>
     <row r="208">
-      <c r="A208" s="5">
+      <c r="A208" s="7">
         <v>43585.852669586653</v>
       </c>
       <c r="B208">
@@ -2046,7 +2050,7 @@
       </c>
     </row>
     <row r="209">
-      <c r="A209" s="5">
+      <c r="A209" s="7">
         <v>43585.852679247386</v>
       </c>
       <c r="B209">
@@ -2054,7 +2058,7 @@
       </c>
     </row>
     <row r="210">
-      <c r="A210" s="5">
+      <c r="A210" s="7">
         <v>43585.85269259545</v>
       </c>
       <c r="B210">
@@ -2062,7 +2066,7 @@
       </c>
     </row>
     <row r="211">
-      <c r="A211" s="5">
+      <c r="A211" s="7">
         <v>43585.852706260048</v>
       </c>
       <c r="B211">
@@ -2070,7 +2074,7 @@
       </c>
     </row>
     <row r="212">
-      <c r="A212" s="5">
+      <c r="A212" s="7">
         <v>43585.852712113294</v>
       </c>
       <c r="B212">
@@ -2078,7 +2082,7 @@
       </c>
     </row>
     <row r="213">
-      <c r="A213" s="5">
+      <c r="A213" s="7">
         <v>43585.852718293667</v>
       </c>
       <c r="B213">
@@ -2086,7 +2090,7 @@
       </c>
     </row>
     <row r="214">
-      <c r="A214" s="5">
+      <c r="A214" s="7">
         <v>43585.852725610952</v>
       </c>
       <c r="B214">
@@ -2094,7 +2098,7 @@
       </c>
     </row>
     <row r="215">
-      <c r="A215" s="5">
+      <c r="A215" s="7">
         <v>43585.852740294184</v>
       </c>
       <c r="B215">
@@ -2102,7 +2106,7 @@
       </c>
     </row>
     <row r="216">
-      <c r="A216" s="5">
+      <c r="A216" s="7">
         <v>43585.852750601363</v>
       </c>
       <c r="B216">
@@ -2110,7 +2114,7 @@
       </c>
     </row>
     <row r="217">
-      <c r="A217" s="5">
+      <c r="A217" s="7">
         <v>43585.852769444929</v>
       </c>
       <c r="B217">
@@ -2118,7 +2122,7 @@
       </c>
     </row>
     <row r="218">
-      <c r="A218" s="5">
+      <c r="A218" s="7">
         <v>43585.852786794538</v>
       </c>
       <c r="B218">
@@ -2126,7 +2130,7 @@
       </c>
     </row>
     <row r="219">
-      <c r="A219" s="5">
+      <c r="A219" s="7">
         <v>43585.852802688954</v>
       </c>
       <c r="B219">
@@ -2134,7 +2138,7 @@
       </c>
     </row>
     <row r="220">
-      <c r="A220" s="5">
+      <c r="A220" s="7">
         <v>43585.852817467181</v>
       </c>
       <c r="B220">
@@ -2142,7 +2146,7 @@
       </c>
     </row>
     <row r="221">
-      <c r="A221" s="5">
+      <c r="A221" s="7">
         <v>43585.852832181961</v>
       </c>
       <c r="B221">
@@ -2150,7 +2154,7 @@
       </c>
     </row>
     <row r="222">
-      <c r="A222" s="5">
+      <c r="A222" s="7">
         <v>43585.852845955291</v>
       </c>
       <c r="B222">
@@ -2158,7 +2162,7 @@
       </c>
     </row>
     <row r="223">
-      <c r="A223" s="5">
+      <c r="A223" s="7">
         <v>43585.852860155283</v>
       </c>
       <c r="B223">
@@ -2166,7 +2170,7 @@
       </c>
     </row>
     <row r="224">
-      <c r="A224" s="5">
+      <c r="A224" s="7">
         <v>43585.852875142475</v>
       </c>
       <c r="B224">
@@ -2174,7 +2178,7 @@
       </c>
     </row>
     <row r="225">
-      <c r="A225" s="5">
+      <c r="A225" s="7">
         <v>43585.852889392641</v>
       </c>
       <c r="B225">
@@ -2182,7 +2186,7 @@
       </c>
     </row>
     <row r="226">
-      <c r="A226" s="5">
+      <c r="A226" s="7">
         <v>43585.852903218241</v>
       </c>
       <c r="B226">
@@ -2190,7 +2194,7 @@
       </c>
     </row>
     <row r="227">
-      <c r="A227" s="5">
+      <c r="A227" s="7">
         <v>43585.852917194716</v>
       </c>
       <c r="B227">
@@ -2198,7 +2202,7 @@
       </c>
     </row>
     <row r="228">
-      <c r="A228" s="5">
+      <c r="A228" s="7">
         <v>43585.852929948363</v>
       </c>
       <c r="B228">
@@ -2206,7 +2210,7 @@
       </c>
     </row>
     <row r="229">
-      <c r="A229" s="5">
+      <c r="A229" s="7">
         <v>43585.852943290374</v>
       </c>
       <c r="B229">
@@ -2214,7 +2218,7 @@
       </c>
     </row>
     <row r="230">
-      <c r="A230" s="5">
+      <c r="A230" s="7">
         <v>43585.852954839473</v>
       </c>
       <c r="B230">
@@ -2222,7 +2226,7 @@
       </c>
     </row>
     <row r="231">
-      <c r="A231" s="5">
+      <c r="A231" s="7">
         <v>43585.852968699532</v>
       </c>
       <c r="B231">
@@ -2230,7 +2234,7 @@
       </c>
     </row>
     <row r="232">
-      <c r="A232" s="5">
+      <c r="A232" s="7">
         <v>43585.8529824781</v>
       </c>
       <c r="B232">
@@ -2238,7 +2242,7 @@
       </c>
     </row>
     <row r="233">
-      <c r="A233" s="5">
+      <c r="A233" s="7">
         <v>43585.852996039437</v>
       </c>
       <c r="B233">
@@ -2246,7 +2250,7 @@
       </c>
     </row>
     <row r="234">
-      <c r="A234" s="5">
+      <c r="A234" s="7">
         <v>43585.85300956259</v>
       </c>
       <c r="B234">
@@ -2254,7 +2258,7 @@
       </c>
     </row>
     <row r="235">
-      <c r="A235" s="5">
+      <c r="A235" s="7">
         <v>43585.853023323114</v>
       </c>
       <c r="B235">
@@ -2262,7 +2266,7 @@
       </c>
     </row>
     <row r="236">
-      <c r="A236" s="5">
+      <c r="A236" s="7">
         <v>43585.853037312627</v>
       </c>
       <c r="B236">
@@ -2270,7 +2274,7 @@
       </c>
     </row>
     <row r="237">
-      <c r="A237" s="5">
+      <c r="A237" s="7">
         <v>43585.8530524167</v>
       </c>
       <c r="B237">
@@ -2278,7 +2282,7 @@
       </c>
     </row>
     <row r="238">
-      <c r="A238" s="5">
+      <c r="A238" s="7">
         <v>43585.853066812851</v>
       </c>
       <c r="B238">
@@ -2286,7 +2290,7 @@
       </c>
     </row>
     <row r="239">
-      <c r="A239" s="5">
+      <c r="A239" s="7">
         <v>43585.853107672767</v>
       </c>
       <c r="B239">
@@ -2294,7 +2298,7 @@
       </c>
     </row>
     <row r="240">
-      <c r="A240" s="5">
+      <c r="A240" s="7">
         <v>43585.853121900233</v>
       </c>
       <c r="B240">
@@ -2302,7 +2306,7 @@
       </c>
     </row>
     <row r="241">
-      <c r="A241" s="5">
+      <c r="A241" s="7">
         <v>43585.853136723395</v>
       </c>
       <c r="B241">
@@ -2310,7 +2314,7 @@
       </c>
     </row>
     <row r="242">
-      <c r="A242" s="5">
+      <c r="A242" s="7">
         <v>43585.853207928129</v>
       </c>
       <c r="B242">
@@ -2318,7 +2322,7 @@
       </c>
     </row>
     <row r="243">
-      <c r="A243" s="5">
+      <c r="A243" s="7">
         <v>43585.853221991099</v>
       </c>
       <c r="B243">
@@ -2326,7 +2330,7 @@
       </c>
     </row>
     <row r="244">
-      <c r="A244" s="5">
+      <c r="A244" s="7">
         <v>43585.853243243997</v>
       </c>
       <c r="B244">
@@ -2334,7 +2338,7 @@
       </c>
     </row>
     <row r="245">
-      <c r="A245" s="5">
+      <c r="A245" s="7">
         <v>43585.853263093391</v>
       </c>
       <c r="B245">
@@ -2342,7 +2346,7 @@
       </c>
     </row>
     <row r="246">
-      <c r="A246" s="5">
+      <c r="A246" s="7">
         <v>43585.853410503943</v>
       </c>
       <c r="B246">
@@ -2350,7 +2354,7 @@
       </c>
     </row>
     <row r="247">
-      <c r="A247" s="5">
+      <c r="A247" s="7">
         <v>43585.853422729648</v>
       </c>
       <c r="B247">
@@ -2358,7 +2362,7 @@
       </c>
     </row>
     <row r="248">
-      <c r="A248" s="5">
+      <c r="A248" s="7">
         <v>43585.853433105513</v>
       </c>
       <c r="B248">
@@ -2366,7 +2370,7 @@
       </c>
     </row>
     <row r="249">
-      <c r="A249" s="5">
+      <c r="A249" s="7">
         <v>43585.853444561129</v>
       </c>
       <c r="B249">
@@ -2374,7 +2378,7 @@
       </c>
     </row>
     <row r="250">
-      <c r="A250" s="5">
+      <c r="A250" s="7">
         <v>43585.853773840587</v>
       </c>
       <c r="B250">
@@ -2382,7 +2386,7 @@
       </c>
     </row>
     <row r="251">
-      <c r="A251" s="5">
+      <c r="A251" s="7">
         <v>43585.853786872001</v>
       </c>
       <c r="B251">
@@ -2390,7 +2394,7 @@
       </c>
     </row>
     <row r="252">
-      <c r="A252" s="5">
+      <c r="A252" s="7">
         <v>43585.85379999526</v>
       </c>
       <c r="B252">
@@ -2398,7 +2402,7 @@
       </c>
     </row>
     <row r="253">
-      <c r="A253" s="5">
+      <c r="A253" s="7">
         <v>43585.854033259675</v>
       </c>
       <c r="B253">
@@ -2406,7 +2410,7 @@
       </c>
     </row>
     <row r="254">
-      <c r="A254" s="5">
+      <c r="A254" s="7">
         <v>43585.854045503656</v>
       </c>
       <c r="B254">
@@ -2414,7 +2418,7 @@
       </c>
     </row>
     <row r="255">
-      <c r="A255" s="5">
+      <c r="A255" s="7">
         <v>43585.854460050352</v>
       </c>
       <c r="B255">
@@ -2422,7 +2426,7 @@
       </c>
     </row>
     <row r="256">
-      <c r="A256" s="5">
+      <c r="A256" s="7">
         <v>43585.854470260558</v>
       </c>
       <c r="B256">
@@ -2430,7 +2434,7 @@
       </c>
     </row>
     <row r="257">
-      <c r="A257" s="5">
+      <c r="A257" s="7">
         <v>43585.854480325128</v>
       </c>
       <c r="B257">
@@ -2438,7 +2442,7 @@
       </c>
     </row>
     <row r="258">
-      <c r="A258" s="5">
+      <c r="A258" s="7">
         <v>43585.854490688769</v>
       </c>
       <c r="B258">
@@ -2446,7 +2450,7 @@
       </c>
     </row>
     <row r="259">
-      <c r="A259" s="5">
+      <c r="A259" s="7">
         <v>43585.85486034397</v>
       </c>
       <c r="B259">
@@ -2454,7 +2458,7 @@
       </c>
     </row>
     <row r="260">
-      <c r="A260" s="5">
+      <c r="A260" s="7">
         <v>43585.854874368873</v>
       </c>
       <c r="B260">
@@ -2462,7 +2466,7 @@
       </c>
     </row>
     <row r="261">
-      <c r="A261" s="5">
+      <c r="A261" s="7">
         <v>43585.854888492031</v>
       </c>
       <c r="B261">
@@ -2470,7 +2474,7 @@
       </c>
     </row>
     <row r="262">
-      <c r="A262" s="5">
+      <c r="A262" s="7">
         <v>43585.854922622442</v>
       </c>
       <c r="B262">
@@ -2478,7 +2482,7 @@
       </c>
     </row>
     <row r="263">
-      <c r="A263" s="5">
+      <c r="A263" s="7">
         <v>43585.854930501315</v>
       </c>
       <c r="B263">
@@ -2486,7 +2490,7 @@
       </c>
     </row>
     <row r="264">
-      <c r="A264" s="5">
+      <c r="A264" s="7">
         <v>43585.854942488717</v>
       </c>
       <c r="B264">
@@ -2494,7 +2498,7 @@
       </c>
     </row>
     <row r="265">
-      <c r="A265" s="5">
+      <c r="A265" s="7">
         <v>43585.854948220658</v>
       </c>
       <c r="B265">
@@ -2502,7 +2506,7 @@
       </c>
     </row>
     <row r="266">
-      <c r="A266" s="5">
+      <c r="A266" s="7">
         <v>43585.854955979979</v>
       </c>
       <c r="B266">
@@ -2510,7 +2514,7 @@
       </c>
     </row>
     <row r="267">
-      <c r="A267" s="5">
+      <c r="A267" s="7">
         <v>43585.854963339749</v>
       </c>
       <c r="B267">
@@ -2518,7 +2522,7 @@
       </c>
     </row>
     <row r="268">
-      <c r="A268" s="5">
+      <c r="A268" s="7">
         <v>43585.854972454261</v>
       </c>
       <c r="B268">
@@ -2526,7 +2530,7 @@
       </c>
     </row>
     <row r="269">
-      <c r="A269" s="5">
+      <c r="A269" s="7">
         <v>43585.854985923623</v>
       </c>
       <c r="B269">
@@ -2534,7 +2538,7 @@
       </c>
     </row>
     <row r="270">
-      <c r="A270" s="5">
+      <c r="A270" s="7">
         <v>43585.85501899221</v>
       </c>
       <c r="B270">
@@ -2542,7 +2546,7 @@
       </c>
     </row>
     <row r="271">
-      <c r="A271" s="5">
+      <c r="A271" s="7">
         <v>43585.855039853603</v>
       </c>
       <c r="B271">
@@ -2550,7 +2554,7 @@
       </c>
     </row>
     <row r="272">
-      <c r="A272" s="5">
+      <c r="A272" s="7">
         <v>43585.85505343636</v>
       </c>
       <c r="B272">
@@ -2558,7 +2562,7 @@
       </c>
     </row>
     <row r="273">
-      <c r="A273" s="5">
+      <c r="A273" s="7">
         <v>43585.85506708303</v>
       </c>
       <c r="B273">
@@ -2566,7 +2570,7 @@
       </c>
     </row>
     <row r="274">
-      <c r="A274" s="5">
+      <c r="A274" s="7">
         <v>43585.855108684045</v>
       </c>
       <c r="B274">
@@ -2574,7 +2578,7 @@
       </c>
     </row>
     <row r="275">
-      <c r="A275" s="5">
+      <c r="A275" s="7">
         <v>43585.855120522661</v>
       </c>
       <c r="B275">
@@ -2582,7 +2586,7 @@
       </c>
     </row>
     <row r="276">
-      <c r="A276" s="5">
+      <c r="A276" s="7">
         <v>43585.85513155302</v>
       </c>
       <c r="B276">
@@ -2590,7 +2594,7 @@
       </c>
     </row>
     <row r="277">
-      <c r="A277" s="5">
+      <c r="A277" s="7">
         <v>43585.855142272194</v>
       </c>
       <c r="B277">
@@ -2598,7 +2602,7 @@
       </c>
     </row>
     <row r="278">
-      <c r="A278" s="5">
+      <c r="A278" s="7">
         <v>43585.855205974542</v>
       </c>
       <c r="B278">
@@ -2606,7 +2610,7 @@
       </c>
     </row>
     <row r="279">
-      <c r="A279" s="5">
+      <c r="A279" s="7">
         <v>43585.856559887303</v>
       </c>
       <c r="B279">
@@ -2614,7 +2618,7 @@
       </c>
     </row>
     <row r="280">
-      <c r="A280" s="5">
+      <c r="A280" s="7">
         <v>43585.856570004835</v>
       </c>
       <c r="B280">
@@ -2622,7 +2626,7 @@
       </c>
     </row>
     <row r="281">
-      <c r="A281" s="5">
+      <c r="A281" s="7">
         <v>43585.856580019114</v>
       </c>
       <c r="B281">
@@ -2630,7 +2634,7 @@
       </c>
     </row>
     <row r="282">
-      <c r="A282" s="5">
+      <c r="A282" s="7">
         <v>43585.856656346237</v>
       </c>
       <c r="B282">
@@ -2638,7 +2642,7 @@
       </c>
     </row>
     <row r="283">
-      <c r="A283" s="5">
+      <c r="A283" s="7">
         <v>43585.856670270558</v>
       </c>
       <c r="B283">
@@ -2646,7 +2650,7 @@
       </c>
     </row>
     <row r="284">
-      <c r="A284" s="5">
+      <c r="A284" s="7">
         <v>43585.856778328773</v>
       </c>
       <c r="B284">
@@ -2654,7 +2658,7 @@
       </c>
     </row>
     <row r="285">
-      <c r="A285" s="5">
+      <c r="A285" s="7">
         <v>43585.85681889439</v>
       </c>
       <c r="B285">
@@ -2662,7 +2666,7 @@
       </c>
     </row>
     <row r="286">
-      <c r="A286" s="5">
+      <c r="A286" s="7">
         <v>43585.85742046708</v>
       </c>
       <c r="B286">
@@ -2670,7 +2674,7 @@
       </c>
     </row>
     <row r="287">
-      <c r="A287" s="5">
+      <c r="A287" s="7">
         <v>43585.857533532311</v>
       </c>
       <c r="B287">
@@ -2678,7 +2682,7 @@
       </c>
     </row>
     <row r="288">
-      <c r="A288" s="5">
+      <c r="A288" s="7">
         <v>43585.857547506108</v>
       </c>
       <c r="B288">
@@ -2686,7 +2690,7 @@
       </c>
     </row>
     <row r="289">
-      <c r="A289" s="5">
+      <c r="A289" s="7">
         <v>43585.857561601675</v>
       </c>
       <c r="B289">
@@ -2694,7 +2698,7 @@
       </c>
     </row>
     <row r="290">
-      <c r="A290" s="5">
+      <c r="A290" s="7">
         <v>43585.857576222508</v>
       </c>
       <c r="B290">
@@ -2702,7 +2706,7 @@
       </c>
     </row>
     <row r="291">
-      <c r="A291" s="5">
+      <c r="A291" s="7">
         <v>43585.857618212234</v>
       </c>
       <c r="B291">
@@ -2710,7 +2714,7 @@
       </c>
     </row>
     <row r="292">
-      <c r="A292" s="5">
+      <c r="A292" s="7">
         <v>43585.857632539468</v>
       </c>
       <c r="B292">
@@ -2718,7 +2722,7 @@
       </c>
     </row>
     <row r="293">
-      <c r="A293" s="5">
+      <c r="A293" s="7">
         <v>43585.857647963334</v>
       </c>
       <c r="B293">
@@ -2726,7 +2730,7 @@
       </c>
     </row>
     <row r="294">
-      <c r="A294" s="5">
+      <c r="A294" s="7">
         <v>43585.857662528404</v>
       </c>
       <c r="B294">
@@ -2734,7 +2738,7 @@
       </c>
     </row>
     <row r="295">
-      <c r="A295" s="5">
+      <c r="A295" s="7">
         <v>43585.857677054591</v>
       </c>
       <c r="B295">
@@ -2742,7 +2746,7 @@
       </c>
     </row>
     <row r="296">
-      <c r="A296" s="5">
+      <c r="A296" s="7">
         <v>43585.857691224664</v>
       </c>
       <c r="B296">
@@ -2750,7 +2754,7 @@
       </c>
     </row>
     <row r="297">
-      <c r="A297" s="5">
+      <c r="A297" s="7">
         <v>43585.857704889029</v>
       </c>
       <c r="B297">
@@ -2758,7 +2762,7 @@
       </c>
     </row>
     <row r="298">
-      <c r="A298" s="5">
+      <c r="A298" s="7">
         <v>43585.857817071024</v>
       </c>
       <c r="B298">
@@ -2766,7 +2770,7 @@
       </c>
     </row>
     <row r="299">
-      <c r="A299" s="5">
+      <c r="A299" s="7">
         <v>43585.857826180552</v>
       </c>
       <c r="B299">
@@ -2774,7 +2778,7 @@
       </c>
     </row>
     <row r="300">
-      <c r="A300" s="5">
+      <c r="A300" s="7">
         <v>43585.857975331135</v>
       </c>
       <c r="B300">
@@ -2782,7 +2786,7 @@
       </c>
     </row>
     <row r="301">
-      <c r="A301" s="5">
+      <c r="A301" s="7">
         <v>43585.857988191769</v>
       </c>
       <c r="B301">
@@ -2790,7 +2794,7 @@
       </c>
     </row>
     <row r="302">
-      <c r="A302" s="5">
+      <c r="A302" s="7">
         <v>43585.858650010305</v>
       </c>
       <c r="B302">
@@ -2798,7 +2802,7 @@
       </c>
     </row>
     <row r="303">
-      <c r="A303" s="5">
+      <c r="A303" s="7">
         <v>43585.858662262559</v>
       </c>
       <c r="B303">
@@ -2806,7 +2810,7 @@
       </c>
     </row>
     <row r="304">
-      <c r="A304" s="5">
+      <c r="A304" s="7">
         <v>43585.85867490666</v>
       </c>
       <c r="B304">
@@ -2814,7 +2818,7 @@
       </c>
     </row>
     <row r="305">
-      <c r="A305" s="5">
+      <c r="A305" s="7">
         <v>43585.858690070105</v>
       </c>
       <c r="B305">
@@ -2822,7 +2826,7 @@
       </c>
     </row>
     <row r="306">
-      <c r="A306" s="5">
+      <c r="A306" s="7">
         <v>43585.858703429345</v>
       </c>
       <c r="B306">
@@ -2830,7 +2834,7 @@
       </c>
     </row>
     <row r="307">
-      <c r="A307" s="5">
+      <c r="A307" s="7">
         <v>43585.858771386564</v>
       </c>
       <c r="B307">
@@ -2838,7 +2842,7 @@
       </c>
     </row>
     <row r="308">
-      <c r="A308" s="5">
+      <c r="A308" s="7">
         <v>43585.858784927288</v>
       </c>
       <c r="B308">
@@ -2846,7 +2850,7 @@
       </c>
     </row>
     <row r="309">
-      <c r="A309" s="5">
+      <c r="A309" s="7">
         <v>43585.858798750218</v>
       </c>
       <c r="B309">
@@ -2854,7 +2858,7 @@
       </c>
     </row>
     <row r="310">
-      <c r="A310" s="5">
+      <c r="A310" s="7">
         <v>43585.858812498744</v>
       </c>
       <c r="B310">
@@ -2862,7 +2866,7 @@
       </c>
     </row>
     <row r="311">
-      <c r="A311" s="5">
+      <c r="A311" s="7">
         <v>43585.858826419688</v>
       </c>
       <c r="B311">
@@ -2870,7 +2874,7 @@
       </c>
     </row>
     <row r="312">
-      <c r="A312" s="5">
+      <c r="A312" s="7">
         <v>43585.858839818626</v>
       </c>
       <c r="B312">
@@ -2878,7 +2882,7 @@
       </c>
     </row>
     <row r="313">
-      <c r="A313" s="5">
+      <c r="A313" s="7">
         <v>43585.858892536024</v>
       </c>
       <c r="B313">
@@ -2886,7 +2890,7 @@
       </c>
     </row>
     <row r="314">
-      <c r="A314" s="5">
+      <c r="A314" s="7">
         <v>43585.858905492933</v>
       </c>
       <c r="B314">
@@ -2894,7 +2898,7 @@
       </c>
     </row>
     <row r="315">
-      <c r="A315" s="5">
+      <c r="A315" s="7">
         <v>43585.858914992423</v>
       </c>
       <c r="B315">
@@ -2902,7 +2906,7 @@
       </c>
     </row>
     <row r="316">
-      <c r="A316" s="5">
+      <c r="A316" s="7">
         <v>43585.859444683301</v>
       </c>
       <c r="B316">
@@ -2910,7 +2914,7 @@
       </c>
     </row>
     <row r="317">
-      <c r="A317" s="5">
+      <c r="A317" s="7">
         <v>43585.859457997838</v>
       </c>
       <c r="B317">
@@ -2918,7 +2922,7 @@
       </c>
     </row>
     <row r="318">
-      <c r="A318" s="5">
+      <c r="A318" s="7">
         <v>43585.859497578233</v>
       </c>
       <c r="B318">
@@ -2926,7 +2930,7 @@
       </c>
     </row>
     <row r="319">
-      <c r="A319" s="5">
+      <c r="A319" s="7">
         <v>43585.859510580194</v>
       </c>
       <c r="B319">
@@ -2934,7 +2938,7 @@
       </c>
     </row>
     <row r="320">
-      <c r="A320" s="5">
+      <c r="A320" s="7">
         <v>43585.859523969906</v>
       </c>
       <c r="B320">
@@ -2942,7 +2946,7 @@
       </c>
     </row>
     <row r="321">
-      <c r="A321" s="5">
+      <c r="A321" s="7">
         <v>43585.859694795334</v>
       </c>
       <c r="B321">
@@ -2950,7 +2954,7 @@
       </c>
     </row>
     <row r="322">
-      <c r="A322" s="5">
+      <c r="A322" s="7">
         <v>43585.859780710191</v>
       </c>
       <c r="B322">
@@ -2958,7 +2962,7 @@
       </c>
     </row>
     <row r="323">
-      <c r="A323" s="5">
+      <c r="A323" s="7">
         <v>43585.859792933334</v>
       </c>
       <c r="B323">
@@ -2966,7 +2970,7 @@
       </c>
     </row>
     <row r="324">
-      <c r="A324" s="5">
+      <c r="A324" s="7">
         <v>43585.860465500853</v>
       </c>
       <c r="B324">
@@ -2974,7 +2978,7 @@
       </c>
     </row>
     <row r="325">
-      <c r="A325" s="5">
+      <c r="A325" s="7">
         <v>43585.860478360439</v>
       </c>
       <c r="B325">
@@ -2982,7 +2986,7 @@
       </c>
     </row>
     <row r="326">
-      <c r="A326" s="5">
+      <c r="A326" s="7">
         <v>43585.860491381609</v>
       </c>
       <c r="B326">
@@ -2990,7 +2994,7 @@
       </c>
     </row>
     <row r="327">
-      <c r="A327" s="5">
+      <c r="A327" s="7">
         <v>43585.860504063887</v>
       </c>
       <c r="B327">
@@ -2998,7 +3002,7 @@
       </c>
     </row>
     <row r="328">
-      <c r="A328" s="5">
+      <c r="A328" s="7">
         <v>43585.86051683058</v>
       </c>
       <c r="B328">
@@ -3006,7 +3010,7 @@
       </c>
     </row>
     <row r="329">
-      <c r="A329" s="5">
+      <c r="A329" s="7">
         <v>43585.861793819116</v>
       </c>
       <c r="B329">
@@ -3014,7 +3018,7 @@
       </c>
     </row>
     <row r="330">
-      <c r="A330" s="5">
+      <c r="A330" s="7">
         <v>43585.862517579808</v>
       </c>
       <c r="B330">
@@ -3022,7 +3026,7 @@
       </c>
     </row>
     <row r="331">
-      <c r="A331" s="5">
+      <c r="A331" s="7">
         <v>43585.862529680948</v>
       </c>
       <c r="B331">
@@ -3030,7 +3034,7 @@
       </c>
     </row>
     <row r="332">
-      <c r="A332" s="5">
+      <c r="A332" s="7">
         <v>43585.862542049843</v>
       </c>
       <c r="B332">
@@ -3038,7 +3042,7 @@
       </c>
     </row>
     <row r="333">
-      <c r="A333" s="5">
+      <c r="A333" s="7">
         <v>43585.862554399762</v>
       </c>
       <c r="B333">
@@ -3046,7 +3050,7 @@
       </c>
     </row>
     <row r="334">
-      <c r="A334" s="5">
+      <c r="A334" s="7">
         <v>43585.862567469478</v>
       </c>
       <c r="B334">
@@ -3054,7 +3058,7 @@
       </c>
     </row>
     <row r="335">
-      <c r="A335" s="5">
+      <c r="A335" s="7">
         <v>43585.862580307992</v>
       </c>
       <c r="B335">
@@ -3062,7 +3066,7 @@
       </c>
     </row>
     <row r="336">
-      <c r="A336" s="5">
+      <c r="A336" s="7">
         <v>43585.862593232887</v>
       </c>
       <c r="B336">
@@ -3070,7 +3074,7 @@
       </c>
     </row>
     <row r="337">
-      <c r="A337" s="5">
+      <c r="A337" s="7">
         <v>43585.862631277298</v>
       </c>
       <c r="B337">
@@ -3078,7 +3082,7 @@
       </c>
     </row>
     <row r="338">
-      <c r="A338" s="5">
+      <c r="A338" s="7">
         <v>43585.862644142238</v>
       </c>
       <c r="B338">
@@ -3086,7 +3090,7 @@
       </c>
     </row>
     <row r="339">
-      <c r="A339" s="5">
+      <c r="A339" s="7">
         <v>43585.862683557672</v>
       </c>
       <c r="B339">
@@ -3094,7 +3098,7 @@
       </c>
     </row>
     <row r="340">
-      <c r="A340" s="5">
+      <c r="A340" s="7">
         <v>43585.862697010394</v>
       </c>
       <c r="B340">
@@ -3102,7 +3106,7 @@
       </c>
     </row>
     <row r="341">
-      <c r="A341" s="5">
+      <c r="A341" s="7">
         <v>43585.862710647634</v>
       </c>
       <c r="B341">
@@ -3110,7 +3114,7 @@
       </c>
     </row>
     <row r="342">
-      <c r="A342" s="5">
+      <c r="A342" s="7">
         <v>43585.86272398755</v>
       </c>
       <c r="B342">
@@ -3118,7 +3122,7 @@
       </c>
     </row>
     <row r="343">
-      <c r="A343" s="5">
+      <c r="A343" s="7">
         <v>43585.862736933981</v>
       </c>
       <c r="B343">
@@ -3126,7 +3130,7 @@
       </c>
     </row>
     <row r="344">
-      <c r="A344" s="5">
+      <c r="A344" s="7">
         <v>43585.862750055734</v>
       </c>
       <c r="B344">
@@ -3134,7 +3138,7 @@
       </c>
     </row>
     <row r="345">
-      <c r="A345" s="5">
+      <c r="A345" s="7">
         <v>43585.862763562007</v>
       </c>
       <c r="B345">
@@ -3142,7 +3146,7 @@
       </c>
     </row>
     <row r="346">
-      <c r="A346" s="5">
+      <c r="A346" s="7">
         <v>43585.862777288996</v>
       </c>
       <c r="B346">
@@ -3150,7 +3154,7 @@
       </c>
     </row>
     <row r="347">
-      <c r="A347" s="5">
+      <c r="A347" s="7">
         <v>43585.862790933112</v>
       </c>
       <c r="B347">
@@ -3158,7 +3162,7 @@
       </c>
     </row>
     <row r="348">
-      <c r="A348" s="5">
+      <c r="A348" s="7">
         <v>43585.862804781296</v>
       </c>
       <c r="B348">
@@ -3166,7 +3170,7 @@
       </c>
     </row>
     <row r="349">
-      <c r="A349" s="5">
+      <c r="A349" s="7">
         <v>43585.862818230642</v>
       </c>
       <c r="B349">
@@ -3174,7 +3178,7 @@
       </c>
     </row>
     <row r="350">
-      <c r="A350" s="5">
+      <c r="A350" s="7">
         <v>43585.862831545528</v>
       </c>
       <c r="B350">
@@ -3182,7 +3186,7 @@
       </c>
     </row>
     <row r="351">
-      <c r="A351" s="5">
+      <c r="A351" s="7">
         <v>43585.863865756197</v>
       </c>
       <c r="B351">
@@ -3190,7 +3194,7 @@
       </c>
     </row>
     <row r="352">
-      <c r="A352" s="5">
+      <c r="A352" s="7">
         <v>43585.863878603326</v>
       </c>
       <c r="B352">
@@ -3198,7 +3202,7 @@
       </c>
     </row>
     <row r="353">
-      <c r="A353" s="5">
+      <c r="A353" s="7">
         <v>43585.863992430735</v>
       </c>
       <c r="B353">
@@ -3206,7 +3210,7 @@
       </c>
     </row>
     <row r="354">
-      <c r="A354" s="5">
+      <c r="A354" s="7">
         <v>43585.864153957926</v>
       </c>
       <c r="B354">
@@ -3214,7 +3218,7 @@
       </c>
     </row>
     <row r="355">
-      <c r="A355" s="5">
+      <c r="A355" s="7">
         <v>43585.864166419837</v>
       </c>
       <c r="B355">
@@ -3222,7 +3226,7 @@
       </c>
     </row>
     <row r="356">
-      <c r="A356" s="5">
+      <c r="A356" s="7">
         <v>43585.864178737393</v>
       </c>
       <c r="B356">
@@ -3230,7 +3234,7 @@
       </c>
     </row>
     <row r="357">
-      <c r="A357" s="5">
+      <c r="A357" s="7">
         <v>43585.864191122353</v>
       </c>
       <c r="B357">
@@ -3238,7 +3242,7 @@
       </c>
     </row>
     <row r="358">
-      <c r="A358" s="5">
+      <c r="A358" s="7">
         <v>43585.86420351034</v>
       </c>
       <c r="B358">
@@ -3246,7 +3250,7 @@
       </c>
     </row>
     <row r="359">
-      <c r="A359" s="5">
+      <c r="A359" s="7">
         <v>43585.864216286805</v>
       </c>
       <c r="B359">
@@ -3254,7 +3258,7 @@
       </c>
     </row>
     <row r="360">
-      <c r="A360" s="5">
+      <c r="A360" s="7">
         <v>43585.864265742712</v>
       </c>
       <c r="B360">
@@ -3262,7 +3266,7 @@
       </c>
     </row>
     <row r="361">
-      <c r="A361" s="5">
+      <c r="A361" s="7">
         <v>43585.864277416724</v>
       </c>
       <c r="B361">
@@ -3270,7 +3274,7 @@
       </c>
     </row>
     <row r="362">
-      <c r="A362" s="5">
+      <c r="A362" s="7">
         <v>43585.864337215899</v>
       </c>
       <c r="B362">
@@ -3278,7 +3282,7 @@
       </c>
     </row>
     <row r="363">
-      <c r="A363" s="5">
+      <c r="A363" s="7">
         <v>43585.864417577628</v>
       </c>
       <c r="B363">
@@ -3286,7 +3290,7 @@
       </c>
     </row>
     <row r="364">
-      <c r="A364" s="5">
+      <c r="A364" s="7">
         <v>43585.864884852432</v>
       </c>
       <c r="B364">
@@ -3294,7 +3298,7 @@
       </c>
     </row>
     <row r="365">
-      <c r="A365" s="5">
+      <c r="A365" s="7">
         <v>43585.864920298911</v>
       </c>
       <c r="B365">
@@ -3302,7 +3306,7 @@
       </c>
     </row>
     <row r="366">
-      <c r="A366" s="5">
+      <c r="A366" s="7">
         <v>43585.864932231139</v>
       </c>
       <c r="B366">
@@ -3310,7 +3314,7 @@
       </c>
     </row>
     <row r="367">
-      <c r="A367" s="5">
+      <c r="A367" s="7">
         <v>43585.864944349276</v>
       </c>
       <c r="B367">
@@ -3318,7 +3322,7 @@
       </c>
     </row>
     <row r="368">
-      <c r="A368" s="5">
+      <c r="A368" s="7">
         <v>43585.864991172566</v>
       </c>
       <c r="B368">
@@ -3326,7 +3330,7 @@
       </c>
     </row>
     <row r="369">
-      <c r="A369" s="5">
+      <c r="A369" s="7">
         <v>43585.865003076848</v>
       </c>
       <c r="B369">
@@ -3334,7 +3338,7 @@
       </c>
     </row>
     <row r="370">
-      <c r="A370" s="5">
+      <c r="A370" s="7">
         <v>43585.866400962695</v>
       </c>
       <c r="B370">
@@ -3342,7 +3346,7 @@
       </c>
     </row>
     <row r="371">
-      <c r="A371" s="5">
+      <c r="A371" s="7">
         <v>43585.866412680014</v>
       </c>
       <c r="B371">
@@ -3350,7 +3354,7 @@
       </c>
     </row>
     <row r="372">
-      <c r="A372" s="5">
+      <c r="A372" s="7">
         <v>43585.866423963569</v>
       </c>
       <c r="B372">
@@ -3358,7 +3362,7 @@
       </c>
     </row>
     <row r="373">
-      <c r="A373" s="5">
+      <c r="A373" s="7">
         <v>43585.866435891134</v>
       </c>
       <c r="B373">
@@ -3366,7 +3370,7 @@
       </c>
     </row>
     <row r="374">
-      <c r="A374" s="5">
+      <c r="A374" s="7">
         <v>43585.866571657243</v>
       </c>
       <c r="B374">
@@ -3374,7 +3378,7 @@
       </c>
     </row>
     <row r="375">
-      <c r="A375" s="5">
+      <c r="A375" s="7">
         <v>43585.866582421237</v>
       </c>
       <c r="B375">
@@ -3382,7 +3386,7 @@
       </c>
     </row>
     <row r="376">
-      <c r="A376" s="5">
+      <c r="A376" s="7">
         <v>43585.8665930184</v>
       </c>
       <c r="B376">
@@ -3390,7 +3394,7 @@
       </c>
     </row>
     <row r="377">
-      <c r="A377" s="5">
+      <c r="A377" s="7">
         <v>43585.866607847391</v>
       </c>
       <c r="B377">
@@ -3398,7 +3402,7 @@
       </c>
     </row>
     <row r="378">
-      <c r="A378" s="5">
+      <c r="A378" s="7">
         <v>43585.866621159134</v>
       </c>
       <c r="B378">
@@ -3406,7 +3410,7 @@
       </c>
     </row>
     <row r="379">
-      <c r="A379" s="5">
+      <c r="A379" s="7">
         <v>43585.866658528685</v>
       </c>
       <c r="B379">
@@ -3414,7 +3418,7 @@
       </c>
     </row>
     <row r="380">
-      <c r="A380" s="5">
+      <c r="A380" s="7">
         <v>43585.868175319978</v>
       </c>
       <c r="B380">
@@ -3422,7 +3426,7 @@
       </c>
     </row>
     <row r="381">
-      <c r="A381" s="5">
+      <c r="A381" s="7">
         <v>43585.868765299907</v>
       </c>
       <c r="B381">
@@ -3430,7 +3434,7 @@
       </c>
     </row>
     <row r="382">
-      <c r="A382" s="5">
+      <c r="A382" s="7">
         <v>43585.868876191671</v>
       </c>
       <c r="B382">
@@ -3438,7 +3442,7 @@
       </c>
     </row>
     <row r="383">
-      <c r="A383" s="5">
+      <c r="A383" s="7">
         <v>43585.868889361736</v>
       </c>
       <c r="B383">
@@ -3446,7 +3450,7 @@
       </c>
     </row>
     <row r="384">
-      <c r="A384" s="5">
+      <c r="A384" s="7">
         <v>43585.868902442977</v>
       </c>
       <c r="B384">
@@ -3454,7 +3458,7 @@
       </c>
     </row>
     <row r="385">
-      <c r="A385" s="5">
+      <c r="A385" s="7">
         <v>43585.868915249244</v>
       </c>
       <c r="B385">
@@ -3462,7 +3466,7 @@
       </c>
     </row>
     <row r="386">
-      <c r="A386" s="5">
+      <c r="A386" s="7">
         <v>43585.868955136626</v>
       </c>
       <c r="B386">
@@ -3470,7 +3474,7 @@
       </c>
     </row>
     <row r="387">
-      <c r="A387" s="5">
+      <c r="A387" s="7">
         <v>43585.868995557306</v>
       </c>
       <c r="B387">
@@ -3478,7 +3482,7 @@
       </c>
     </row>
     <row r="388">
-      <c r="A388" s="5">
+      <c r="A388" s="7">
         <v>43585.869007512694</v>
       </c>
       <c r="B388">
@@ -3486,7 +3490,7 @@
       </c>
     </row>
     <row r="389">
-      <c r="A389" s="5">
+      <c r="A389" s="7">
         <v>43585.869960193755</v>
       </c>
       <c r="B389">
@@ -3494,7 +3498,7 @@
       </c>
     </row>
     <row r="390">
-      <c r="A390" s="5">
+      <c r="A390" s="7">
         <v>43585.869967904408</v>
       </c>
       <c r="B390">
@@ -3502,7 +3506,7 @@
       </c>
     </row>
     <row r="391">
-      <c r="A391" s="5">
+      <c r="A391" s="7">
         <v>43585.86998362618</v>
       </c>
       <c r="B391">
@@ -3510,7 +3514,7 @@
       </c>
     </row>
     <row r="392">
-      <c r="A392" s="5">
+      <c r="A392" s="7">
         <v>43585.869999455637</v>
       </c>
       <c r="B392">
@@ -3518,7 +3522,7 @@
       </c>
     </row>
     <row r="393">
-      <c r="A393" s="5">
+      <c r="A393" s="7">
         <v>43585.870015240507</v>
       </c>
       <c r="B393">
@@ -3526,7 +3530,7 @@
       </c>
     </row>
     <row r="394">
-      <c r="A394" s="5">
+      <c r="A394" s="7">
         <v>43585.870031085447</v>
       </c>
       <c r="B394">
@@ -3534,7 +3538,7 @@
       </c>
     </row>
     <row r="395">
-      <c r="A395" s="5">
+      <c r="A395" s="7">
         <v>43585.870047150769</v>
       </c>
       <c r="B395">
@@ -3542,7 +3546,7 @@
       </c>
     </row>
     <row r="396">
-      <c r="A396" s="5">
+      <c r="A396" s="7">
         <v>43585.870063672541</v>
       </c>
       <c r="B396">
@@ -3550,7 +3554,7 @@
       </c>
     </row>
     <row r="397">
-      <c r="A397" s="5">
+      <c r="A397" s="7">
         <v>43585.870077632608</v>
       </c>
       <c r="B397">
@@ -3558,7 +3562,7 @@
       </c>
     </row>
     <row r="398">
-      <c r="A398" s="5">
+      <c r="A398" s="7">
         <v>43585.870088508818</v>
       </c>
       <c r="B398">
@@ -3566,7 +3570,7 @@
       </c>
     </row>
     <row r="399">
-      <c r="A399" s="5">
+      <c r="A399" s="7">
         <v>43585.870098131942</v>
       </c>
       <c r="B399">
@@ -3574,7 +3578,7 @@
       </c>
     </row>
     <row r="400">
-      <c r="A400" s="5">
+      <c r="A400" s="7">
         <v>43585.870144068263</v>
       </c>
       <c r="B400">
@@ -3582,7 +3586,7 @@
       </c>
     </row>
     <row r="401">
-      <c r="A401" s="5">
+      <c r="A401" s="7">
         <v>43585.870153893717</v>
       </c>
       <c r="B401">
@@ -3590,7 +3594,7 @@
       </c>
     </row>
     <row r="402">
-      <c r="A402" s="5">
+      <c r="A402" s="7">
         <v>43585.870163701242</v>
       </c>
       <c r="B402">
@@ -3598,7 +3602,7 @@
       </c>
     </row>
     <row r="403">
-      <c r="A403" s="5">
+      <c r="A403" s="7">
         <v>43585.870172978379</v>
       </c>
       <c r="B403">
@@ -3606,7 +3610,7 @@
       </c>
     </row>
     <row r="404">
-      <c r="A404" s="5">
+      <c r="A404" s="7">
         <v>43585.870692375356</v>
       </c>
       <c r="B404">
@@ -3614,7 +3618,7 @@
       </c>
     </row>
     <row r="405">
-      <c r="A405" s="5">
+      <c r="A405" s="7">
         <v>43585.872242157115</v>
       </c>
       <c r="B405">
@@ -3622,7 +3626,7 @@
       </c>
     </row>
     <row r="406">
-      <c r="A406" s="5">
+      <c r="A406" s="7">
         <v>43585.872258281801</v>
       </c>
       <c r="B406">
@@ -3630,7 +3634,7 @@
       </c>
     </row>
     <row r="407">
-      <c r="A407" s="5">
+      <c r="A407" s="7">
         <v>43585.873941503582</v>
       </c>
       <c r="B407">
@@ -3638,7 +3642,7 @@
       </c>
     </row>
     <row r="408">
-      <c r="A408" s="5">
+      <c r="A408" s="7">
         <v>43585.876425618189</v>
       </c>
       <c r="B408">
@@ -3646,7 +3650,7 @@
       </c>
     </row>
     <row r="409">
-      <c r="A409" s="5">
+      <c r="A409" s="7">
         <v>43585.876461243839</v>
       </c>
       <c r="B409">
@@ -3654,7 +3658,7 @@
       </c>
     </row>
     <row r="410">
-      <c r="A410" s="5">
+      <c r="A410" s="7">
         <v>43585.876553822542</v>
       </c>
       <c r="B410">
@@ -3662,7 +3666,7 @@
       </c>
     </row>
     <row r="411">
-      <c r="A411" s="5">
+      <c r="A411" s="7">
         <v>43585.876565477818</v>
       </c>
       <c r="B411">
@@ -3670,7 +3674,7 @@
       </c>
     </row>
     <row r="412">
-      <c r="A412" s="5">
+      <c r="A412" s="7">
         <v>43585.876577243907</v>
       </c>
       <c r="B412">
@@ -3678,7 +3682,7 @@
       </c>
     </row>
     <row r="413">
-      <c r="A413" s="5">
+      <c r="A413" s="7">
         <v>43585.87658882339</v>
       </c>
       <c r="B413">
@@ -3686,7 +3690,7 @@
       </c>
     </row>
     <row r="414">
-      <c r="A414" s="5">
+      <c r="A414" s="7">
         <v>43585.876600732096</v>
       </c>
       <c r="B414">
@@ -3694,7 +3698,7 @@
       </c>
     </row>
     <row r="415">
-      <c r="A415" s="5">
+      <c r="A415" s="7">
         <v>43585.876612811699</v>
       </c>
       <c r="B415">
@@ -3702,7 +3706,7 @@
       </c>
     </row>
     <row r="416">
-      <c r="A416" s="5">
+      <c r="A416" s="7">
         <v>43585.876625082106</v>
       </c>
       <c r="B416">
@@ -3710,7 +3714,7 @@
       </c>
     </row>
     <row r="417">
-      <c r="A417" s="5">
+      <c r="A417" s="7">
         <v>43585.876687734271</v>
       </c>
       <c r="B417">
@@ -3718,7 +3722,7 @@
       </c>
     </row>
     <row r="418">
-      <c r="A418" s="5">
+      <c r="A418" s="7">
         <v>43585.876700398512</v>
       </c>
       <c r="B418">
@@ -3726,7 +3730,7 @@
       </c>
     </row>
     <row r="419">
-      <c r="A419" s="5">
+      <c r="A419" s="7">
         <v>43585.876712832833</v>
       </c>
       <c r="B419">
@@ -3734,7 +3738,7 @@
       </c>
     </row>
     <row r="420">
-      <c r="A420" s="5">
+      <c r="A420" s="7">
         <v>43585.878880354925</v>
       </c>
       <c r="B420">
@@ -3742,7 +3746,7 @@
       </c>
     </row>
     <row r="421">
-      <c r="A421" s="5">
+      <c r="A421" s="7">
         <v>43585.878889504587</v>
       </c>
       <c r="B421">
@@ -3750,7 +3754,7 @@
       </c>
     </row>
     <row r="422">
-      <c r="A422" s="5">
+      <c r="A422" s="7">
         <v>43585.878898682771</v>
       </c>
       <c r="B422">
@@ -3758,7 +3762,7 @@
       </c>
     </row>
     <row r="423">
-      <c r="A423" s="5">
+      <c r="A423" s="7">
         <v>43585.879844700568</v>
       </c>
       <c r="B423">
@@ -3766,7 +3770,7 @@
       </c>
     </row>
     <row r="424">
-      <c r="A424" s="5">
+      <c r="A424" s="7">
         <v>43585.879858390079</v>
       </c>
       <c r="B424">
@@ -3774,7 +3778,7 @@
       </c>
     </row>
     <row r="425">
-      <c r="A425" s="5">
+      <c r="A425" s="7">
         <v>43585.880121607217</v>
       </c>
       <c r="B425">
@@ -3782,7 +3786,7 @@
       </c>
     </row>
     <row r="426">
-      <c r="A426" s="5">
+      <c r="A426" s="7">
         <v>43585.880130645237</v>
       </c>
       <c r="B426">
@@ -3790,7 +3794,7 @@
       </c>
     </row>
     <row r="427">
-      <c r="A427" s="5">
+      <c r="A427" s="7">
         <v>43585.88051183091</v>
       </c>
       <c r="B427">
@@ -3798,7 +3802,7 @@
       </c>
     </row>
     <row r="428">
-      <c r="A428" s="5">
+      <c r="A428" s="7">
         <v>43585.880521869753</v>
       </c>
       <c r="B428">
@@ -3806,7 +3810,7 @@
       </c>
     </row>
     <row r="429">
-      <c r="A429" s="5">
+      <c r="A429" s="7">
         <v>43585.880531725823</v>
       </c>
       <c r="B429">
@@ -3814,7 +3818,7 @@
       </c>
     </row>
     <row r="430">
-      <c r="A430" s="5">
+      <c r="A430" s="7">
         <v>43585.880599927739</v>
       </c>
       <c r="B430">
@@ -3822,7 +3826,7 @@
       </c>
     </row>
     <row r="431">
-      <c r="A431" s="5">
+      <c r="A431" s="7">
         <v>43585.880609382293</v>
       </c>
       <c r="B431">
@@ -3830,7 +3834,7 @@
       </c>
     </row>
     <row r="432">
-      <c r="A432" s="5">
+      <c r="A432" s="7">
         <v>43585.880632221466</v>
       </c>
       <c r="B432">
@@ -3838,7 +3842,7 @@
       </c>
     </row>
     <row r="433">
-      <c r="A433" s="5">
+      <c r="A433" s="7">
         <v>43585.880646377685</v>
       </c>
       <c r="B433">
@@ -3846,7 +3850,7 @@
       </c>
     </row>
     <row r="434">
-      <c r="A434" s="5">
+      <c r="A434" s="7">
         <v>43585.880659259157</v>
       </c>
       <c r="B434">
@@ -3854,7 +3858,7 @@
       </c>
     </row>
     <row r="435">
-      <c r="A435" s="5">
+      <c r="A435" s="7">
         <v>43585.88067106728</v>
       </c>
       <c r="B435">
@@ -3862,7 +3866,7 @@
       </c>
     </row>
     <row r="436">
-      <c r="A436" s="5">
+      <c r="A436" s="7">
         <v>43585.880727611257</v>
       </c>
       <c r="B436">
@@ -3870,7 +3874,7 @@
       </c>
     </row>
     <row r="437">
-      <c r="A437" s="5">
+      <c r="A437" s="7">
         <v>43585.880747992545</v>
       </c>
       <c r="B437">
@@ -3878,7 +3882,7 @@
       </c>
     </row>
     <row r="438">
-      <c r="A438" s="5">
+      <c r="A438" s="7">
         <v>43585.880760697182</v>
       </c>
       <c r="B438">
@@ -3886,7 +3890,7 @@
       </c>
     </row>
     <row r="439">
-      <c r="A439" s="5">
+      <c r="A439" s="7">
         <v>43585.880775576574</v>
       </c>
       <c r="B439">
@@ -3894,7 +3898,7 @@
       </c>
     </row>
     <row r="440">
-      <c r="A440" s="5">
+      <c r="A440" s="7">
         <v>43585.880786083057</v>
       </c>
       <c r="B440">
@@ -3902,7 +3906,7 @@
       </c>
     </row>
     <row r="441">
-      <c r="A441" s="5">
+      <c r="A441" s="7">
         <v>43585.880796826095</v>
       </c>
       <c r="B441">
@@ -3910,7 +3914,7 @@
       </c>
     </row>
     <row r="442">
-      <c r="A442" s="5">
+      <c r="A442" s="7">
         <v>43585.880808414542</v>
       </c>
       <c r="B442">
@@ -3918,7 +3922,7 @@
       </c>
     </row>
     <row r="443">
-      <c r="A443" s="5">
+      <c r="A443" s="7">
         <v>43585.880828637048</v>
       </c>
       <c r="B443">
@@ -3926,7 +3930,7 @@
       </c>
     </row>
     <row r="444">
-      <c r="A444" s="5">
+      <c r="A444" s="7">
         <v>43585.880838164594</v>
       </c>
       <c r="B444">
@@ -3934,7 +3938,7 @@
       </c>
     </row>
     <row r="445">
-      <c r="A445" s="5">
+      <c r="A445" s="7">
         <v>43585.880857884302</v>
       </c>
       <c r="B445">
@@ -3942,7 +3946,7 @@
       </c>
     </row>
     <row r="446">
-      <c r="A446" s="5">
+      <c r="A446" s="7">
         <v>43585.880868053413</v>
       </c>
       <c r="B446">
@@ -3950,7 +3954,7 @@
       </c>
     </row>
     <row r="447">
-      <c r="A447" s="5">
+      <c r="A447" s="7">
         <v>43585.880877837539</v>
       </c>
       <c r="B447">
@@ -3958,7 +3962,7 @@
       </c>
     </row>
     <row r="448">
-      <c r="A448" s="5">
+      <c r="A448" s="7">
         <v>43585.8808889176</v>
       </c>
       <c r="B448">
@@ -3966,7 +3970,7 @@
       </c>
     </row>
     <row r="449">
-      <c r="A449" s="5">
+      <c r="A449" s="7">
         <v>43585.882339876494</v>
       </c>
       <c r="B449">
@@ -3974,7 +3978,7 @@
       </c>
     </row>
     <row r="450">
-      <c r="A450" s="5">
+      <c r="A450" s="7">
         <v>43585.882345417049</v>
       </c>
       <c r="B450">
@@ -3982,7 +3986,7 @@
       </c>
     </row>
     <row r="451">
-      <c r="A451" s="5">
+      <c r="A451" s="7">
         <v>43585.882351044216</v>
       </c>
       <c r="B451">
@@ -3990,7 +3994,7 @@
       </c>
     </row>
     <row r="452">
-      <c r="A452" s="5">
+      <c r="A452" s="7">
         <v>43585.882356702234</v>
       </c>
       <c r="B452">
@@ -3998,7 +4002,7 @@
       </c>
     </row>
     <row r="453">
-      <c r="A453" s="5">
+      <c r="A453" s="7">
         <v>43585.882362479228</v>
       </c>
       <c r="B453">
@@ -4006,7 +4010,7 @@
       </c>
     </row>
     <row r="454">
-      <c r="A454" s="5">
+      <c r="A454" s="7">
         <v>43585.882368391729</v>
       </c>
       <c r="B454">
@@ -4014,7 +4018,7 @@
       </c>
     </row>
     <row r="455">
-      <c r="A455" s="5">
+      <c r="A455" s="7">
         <v>43585.882374317735</v>
       </c>
       <c r="B455">
@@ -4022,7 +4026,7 @@
       </c>
     </row>
     <row r="456">
-      <c r="A456" s="5">
+      <c r="A456" s="7">
         <v>43585.882380423951</v>
       </c>
       <c r="B456">
@@ -4030,7 +4034,7 @@
       </c>
     </row>
     <row r="457">
-      <c r="A457" s="5">
+      <c r="A457" s="7">
         <v>43585.882386709207</v>
       </c>
       <c r="B457">
@@ -4038,7 +4042,7 @@
       </c>
     </row>
     <row r="458">
-      <c r="A458" s="5">
+      <c r="A458" s="7">
         <v>43585.882480918779</v>
       </c>
       <c r="B458">
@@ -4046,7 +4050,7 @@
       </c>
     </row>
     <row r="459">
-      <c r="A459" s="5">
+      <c r="A459" s="7">
         <v>43585.882486805436</v>
       </c>
       <c r="B459">
@@ -4054,7 +4058,7 @@
       </c>
     </row>
     <row r="460">
-      <c r="A460" s="5">
+      <c r="A460" s="7">
         <v>43585.882492522003</v>
       </c>
       <c r="B460">
@@ -4062,7 +4066,7 @@
       </c>
     </row>
     <row r="461">
-      <c r="A461" s="5">
+      <c r="A461" s="7">
         <v>43585.882664305274</v>
       </c>
       <c r="B461">
@@ -4070,7 +4074,7 @@
       </c>
     </row>
     <row r="462">
-      <c r="A462" s="5">
+      <c r="A462" s="7">
         <v>43585.882670370163</v>
       </c>
       <c r="B462">
@@ -4078,7 +4082,7 @@
       </c>
     </row>
     <row r="463">
-      <c r="A463" s="5">
+      <c r="A463" s="7">
         <v>43585.88267638383</v>
       </c>
       <c r="B463">
@@ -4086,7 +4090,7 @@
       </c>
     </row>
     <row r="464">
-      <c r="A464" s="5">
+      <c r="A464" s="7">
         <v>43585.882682525909</v>
       </c>
       <c r="B464">
@@ -4094,7 +4098,7 @@
       </c>
     </row>
     <row r="465">
-      <c r="A465" s="5">
+      <c r="A465" s="7">
         <v>43585.882688894984</v>
       </c>
       <c r="B465">
@@ -4102,7 +4106,7 @@
       </c>
     </row>
     <row r="466">
-      <c r="A466" s="5">
+      <c r="A466" s="7">
         <v>43585.88269560854</v>
       </c>
       <c r="B466">
@@ -4110,7 +4114,7 @@
       </c>
     </row>
     <row r="467">
-      <c r="A467" s="5">
+      <c r="A467" s="7">
         <v>43585.882702459814</v>
       </c>
       <c r="B467">
@@ -4118,7 +4122,7 @@
       </c>
     </row>
     <row r="468">
-      <c r="A468" s="5">
+      <c r="A468" s="7">
         <v>43585.882945031393</v>
       </c>
       <c r="B468">
@@ -4126,7 +4130,7 @@
       </c>
     </row>
     <row r="469">
-      <c r="A469" s="5">
+      <c r="A469" s="7">
         <v>43585.882954675122</v>
       </c>
       <c r="B469">
@@ -4134,7 +4138,7 @@
       </c>
     </row>
     <row r="470">
-      <c r="A470" s="5">
+      <c r="A470" s="7">
         <v>43585.882964369957</v>
       </c>
       <c r="B470">
@@ -4142,7 +4146,7 @@
       </c>
     </row>
     <row r="471">
-      <c r="A471" s="5">
+      <c r="A471" s="7">
         <v>43585.883602864349</v>
       </c>
       <c r="B471">
@@ -4150,7 +4154,7 @@
       </c>
     </row>
     <row r="472">
-      <c r="A472" s="5">
+      <c r="A472" s="7">
         <v>43585.883812579676</v>
       </c>
       <c r="B472">
@@ -4158,7 +4162,7 @@
       </c>
     </row>
     <row r="473">
-      <c r="A473" s="5">
+      <c r="A473" s="7">
         <v>43585.883823111079</v>
       </c>
       <c r="B473">
@@ -4166,7 +4170,7 @@
       </c>
     </row>
     <row r="474">
-      <c r="A474" s="5">
+      <c r="A474" s="7">
         <v>43585.884944500052</v>
       </c>
       <c r="B474">
@@ -4174,7 +4178,7 @@
       </c>
     </row>
     <row r="475">
-      <c r="A475" s="5">
+      <c r="A475" s="7">
         <v>43585.884967647726</v>
       </c>
       <c r="B475">
@@ -4182,7 +4186,7 @@
       </c>
     </row>
     <row r="476">
-      <c r="A476" s="5">
+      <c r="A476" s="7">
         <v>43585.884979910683</v>
       </c>
       <c r="B476">
@@ -4190,7 +4194,7 @@
       </c>
     </row>
     <row r="477">
-      <c r="A477" s="5">
+      <c r="A477" s="7">
         <v>43585.884990521481</v>
       </c>
       <c r="B477">
@@ -4198,7 +4202,7 @@
       </c>
     </row>
     <row r="478">
-      <c r="A478" s="5">
+      <c r="A478" s="7">
         <v>43585.88557539566</v>
       </c>
       <c r="B478">
@@ -4206,7 +4210,7 @@
       </c>
     </row>
     <row r="479">
-      <c r="A479" s="5">
+      <c r="A479" s="7">
         <v>43585.88587403053</v>
       </c>
       <c r="B479">
@@ -4214,7 +4218,7 @@
       </c>
     </row>
     <row r="480">
-      <c r="A480" s="5">
+      <c r="A480" s="7">
         <v>43585.88588232547</v>
       </c>
       <c r="B480">
@@ -4222,7 +4226,7 @@
       </c>
     </row>
     <row r="481">
-      <c r="A481" s="5">
+      <c r="A481" s="7">
         <v>43585.88589789765</v>
       </c>
       <c r="B481">
@@ -4230,7 +4234,7 @@
       </c>
     </row>
     <row r="482">
-      <c r="A482" s="5">
+      <c r="A482" s="7">
         <v>43585.885906253126</v>
       </c>
       <c r="B482">
@@ -4238,7 +4242,7 @@
       </c>
     </row>
     <row r="483">
-      <c r="A483" s="5">
+      <c r="A483" s="7">
         <v>43585.885914561921</v>
       </c>
       <c r="B483">
@@ -4246,7 +4250,7 @@
       </c>
     </row>
     <row r="484">
-      <c r="A484" s="5">
+      <c r="A484" s="7">
         <v>43585.885922768968</v>
       </c>
       <c r="B484">
@@ -4254,7 +4258,7 @@
       </c>
     </row>
     <row r="485">
-      <c r="A485" s="5">
+      <c r="A485" s="7">
         <v>43585.886649533524</v>
       </c>
       <c r="B485">
@@ -4262,7 +4266,7 @@
       </c>
     </row>
     <row r="486">
-      <c r="A486" s="5">
+      <c r="A486" s="7">
         <v>43585.887940897723</v>
       </c>
       <c r="B486">
@@ -4270,7 +4274,7 @@
       </c>
     </row>
     <row r="487">
-      <c r="A487" s="5">
+      <c r="A487" s="7">
         <v>43585.88794892095</v>
       </c>
       <c r="B487">
@@ -4278,7 +4282,7 @@
       </c>
     </row>
     <row r="488">
-      <c r="A488" s="5">
+      <c r="A488" s="7">
         <v>43585.888592472998</v>
       </c>
       <c r="B488">
@@ -4286,7 +4290,7 @@
       </c>
     </row>
     <row r="489">
-      <c r="A489" s="5">
+      <c r="A489" s="7">
         <v>43585.888600559905</v>
       </c>
       <c r="B489">
@@ -4294,7 +4298,7 @@
       </c>
     </row>
     <row r="490">
-      <c r="A490" s="5">
+      <c r="A490" s="7">
         <v>43585.888608532958</v>
       </c>
       <c r="B490">
@@ -4302,7 +4306,7 @@
       </c>
     </row>
     <row r="491">
-      <c r="A491" s="5">
+      <c r="A491" s="7">
         <v>43585.889025987475</v>
       </c>
       <c r="B491">
@@ -4310,7 +4314,7 @@
       </c>
     </row>
     <row r="492">
-      <c r="A492" s="5">
+      <c r="A492" s="7">
         <v>43585.889035434113</v>
       </c>
       <c r="B492">
@@ -4318,7 +4322,7 @@
       </c>
     </row>
     <row r="493">
-      <c r="A493" s="5">
+      <c r="A493" s="7">
         <v>43585.889092092526</v>
       </c>
       <c r="B493">
@@ -4326,7 +4330,7 @@
       </c>
     </row>
     <row r="494">
-      <c r="A494" s="5">
+      <c r="A494" s="7">
         <v>43585.889099470449</v>
       </c>
       <c r="B494">
@@ -4334,7 +4338,7 @@
       </c>
     </row>
     <row r="495">
-      <c r="A495" s="5">
+      <c r="A495" s="7">
         <v>43585.892026423477</v>
       </c>
       <c r="B495">
@@ -4342,7 +4346,7 @@
       </c>
     </row>
     <row r="496">
-      <c r="A496" s="5">
+      <c r="A496" s="7">
         <v>43585.892035417259</v>
       </c>
       <c r="B496">
@@ -4350,7 +4354,7 @@
       </c>
     </row>
     <row r="497">
-      <c r="A497" s="5">
+      <c r="A497" s="7">
         <v>43585.892044453773</v>
       </c>
       <c r="B497">
@@ -4358,7 +4362,7 @@
       </c>
     </row>
     <row r="498">
-      <c r="A498" s="5">
+      <c r="A498" s="7">
         <v>43585.892274129554</v>
       </c>
       <c r="B498">
@@ -4366,7 +4370,7 @@
       </c>
     </row>
     <row r="499">
-      <c r="A499" s="5">
+      <c r="A499" s="7">
         <v>43585.892540049041</v>
       </c>
       <c r="B499">
@@ -4374,7 +4378,7 @@
       </c>
     </row>
     <row r="500">
-      <c r="A500" s="5">
+      <c r="A500" s="7">
         <v>43585.892552682664</v>
       </c>
       <c r="B500">
@@ -4382,7 +4386,7 @@
       </c>
     </row>
     <row r="501">
-      <c r="A501" s="5">
+      <c r="A501" s="7">
         <v>43585.892565524438</v>
       </c>
       <c r="B501">
@@ -4390,7 +4394,7 @@
       </c>
     </row>
     <row r="502">
-      <c r="A502" s="5">
+      <c r="A502" s="7">
         <v>43585.892578155734</v>
       </c>
       <c r="B502">
@@ -4398,7 +4402,7 @@
       </c>
     </row>
     <row r="503">
-      <c r="A503" s="5">
+      <c r="A503" s="7">
         <v>43585.892590700299</v>
       </c>
       <c r="B503">
@@ -4406,7 +4410,7 @@
       </c>
     </row>
     <row r="504">
-      <c r="A504" s="5">
+      <c r="A504" s="7">
         <v>43585.893237146549</v>
       </c>
       <c r="B504">
@@ -4414,7 +4418,7 @@
       </c>
     </row>
     <row r="505">
-      <c r="A505" s="5">
+      <c r="A505" s="7">
         <v>43585.893725663896</v>
       </c>
       <c r="B505">
@@ -4422,7 +4426,7 @@
       </c>
     </row>
     <row r="506">
-      <c r="A506" s="5">
+      <c r="A506" s="7">
         <v>43585.89374733204</v>
       </c>
       <c r="B506">
@@ -4430,7 +4434,7 @@
       </c>
     </row>
     <row r="507">
-      <c r="A507" s="5">
+      <c r="A507" s="7">
         <v>43585.897644052515</v>
       </c>
       <c r="B507">
@@ -4438,7 +4442,7 @@
       </c>
     </row>
     <row r="508">
-      <c r="A508" s="5">
+      <c r="A508" s="7">
         <v>43585.899268432055</v>
       </c>
       <c r="B508">
@@ -4446,7 +4450,7 @@
       </c>
     </row>
     <row r="509">
-      <c r="A509" s="5">
+      <c r="A509" s="7">
         <v>43585.899333800888</v>
       </c>
       <c r="B509">
@@ -4454,7 +4458,7 @@
       </c>
     </row>
     <row r="510">
-      <c r="A510" s="5">
+      <c r="A510" s="7">
         <v>43585.89934469061</v>
       </c>
       <c r="B510">
@@ -4462,7 +4466,7 @@
       </c>
     </row>
     <row r="511">
-      <c r="A511" s="5">
+      <c r="A511" s="7">
         <v>43585.900675092707</v>
       </c>
       <c r="B511">
@@ -4470,7 +4474,7 @@
       </c>
     </row>
     <row r="512">
-      <c r="A512" s="5">
+      <c r="A512" s="7">
         <v>43585.900685570901</v>
       </c>
       <c r="B512">
@@ -4478,7 +4482,7 @@
       </c>
     </row>
     <row r="513">
-      <c r="A513" s="5">
+      <c r="A513" s="7">
         <v>43585.900696028722</v>
       </c>
       <c r="B513">
@@ -4486,7 +4490,7 @@
       </c>
     </row>
     <row r="514">
-      <c r="A514" s="5">
+      <c r="A514" s="7">
         <v>43585.903040363803</v>
       </c>
       <c r="B514">
@@ -4494,7 +4498,7 @@
       </c>
     </row>
     <row r="515">
-      <c r="A515" s="5">
+      <c r="A515" s="7">
         <v>43585.903050355148</v>
       </c>
       <c r="B515">
@@ -4502,7 +4506,7 @@
       </c>
     </row>
     <row r="516">
-      <c r="A516" s="5">
+      <c r="A516" s="7">
         <v>43585.903060148354</v>
       </c>
       <c r="B516">
@@ -4510,7 +4514,7 @@
       </c>
     </row>
     <row r="517">
-      <c r="A517" s="5">
+      <c r="A517" s="7">
         <v>43585.903069963337</v>
       </c>
       <c r="B517">
@@ -4518,7 +4522,7 @@
       </c>
     </row>
     <row r="518">
-      <c r="A518" s="5">
+      <c r="A518" s="7">
         <v>43585.903079628712</v>
       </c>
       <c r="B518">
@@ -4526,7 +4530,7 @@
       </c>
     </row>
     <row r="519">
-      <c r="A519" s="5">
+      <c r="A519" s="7">
         <v>43585.903089296073</v>
       </c>
       <c r="B519">
@@ -4534,7 +4538,7 @@
       </c>
     </row>
     <row r="520">
-      <c r="A520" s="5">
+      <c r="A520" s="7">
         <v>43585.903098832467</v>
       </c>
       <c r="B520">
@@ -4542,7 +4546,7 @@
       </c>
     </row>
     <row r="521">
-      <c r="A521" s="5">
+      <c r="A521" s="7">
         <v>43585.903108222759</v>
       </c>
       <c r="B521">
@@ -4550,7 +4554,7 @@
       </c>
     </row>
     <row r="522">
-      <c r="A522" s="5">
+      <c r="A522" s="7">
         <v>43585.903117581853</v>
       </c>
       <c r="B522">
@@ -4558,7 +4562,7 @@
       </c>
     </row>
     <row r="523">
-      <c r="A523" s="5">
+      <c r="A523" s="7">
         <v>43585.903126800433</v>
       </c>
       <c r="B523">
@@ -4566,7 +4570,7 @@
       </c>
     </row>
     <row r="524">
-      <c r="A524" s="5">
+      <c r="A524" s="7">
         <v>43585.904237461393</v>
       </c>
       <c r="B524">
@@ -4574,7 +4578,7 @@
       </c>
     </row>
     <row r="525">
-      <c r="A525" s="5">
+      <c r="A525" s="7">
         <v>43585.904250574997</v>
       </c>
       <c r="B525">
@@ -4582,7 +4586,7 @@
       </c>
     </row>
     <row r="526">
-      <c r="A526" s="5">
+      <c r="A526" s="7">
         <v>43585.904438514379</v>
       </c>
       <c r="B526">
@@ -4590,7 +4594,7 @@
       </c>
     </row>
     <row r="527">
-      <c r="A527" s="5">
+      <c r="A527" s="7">
         <v>43585.904450848931</v>
       </c>
       <c r="B527">
@@ -4598,7 +4602,7 @@
       </c>
     </row>
     <row r="528">
-      <c r="A528" s="5">
+      <c r="A528" s="7">
         <v>43585.904464166379</v>
       </c>
       <c r="B528">
@@ -4606,7 +4610,7 @@
       </c>
     </row>
     <row r="529">
-      <c r="A529" s="5">
+      <c r="A529" s="7">
         <v>43585.904477810953</v>
       </c>
       <c r="B529">
@@ -4614,7 +4618,7 @@
       </c>
     </row>
     <row r="530">
-      <c r="A530" s="5">
+      <c r="A530" s="7">
         <v>43585.904490205925</v>
       </c>
       <c r="B530">
@@ -4622,7 +4626,7 @@
       </c>
     </row>
     <row r="531">
-      <c r="A531" s="5">
+      <c r="A531" s="7">
         <v>43585.904503229074</v>
       </c>
       <c r="B531">
@@ -4630,7 +4634,7 @@
       </c>
     </row>
     <row r="532">
-      <c r="A532" s="5">
+      <c r="A532" s="7">
         <v>43585.904515778297</v>
       </c>
       <c r="B532">
@@ -4638,7 +4642,7 @@
       </c>
     </row>
     <row r="533">
-      <c r="A533" s="5">
+      <c r="A533" s="7">
         <v>43585.904528659768</v>
       </c>
       <c r="B533">
@@ -4646,7 +4650,7 @@
       </c>
     </row>
     <row r="534">
-      <c r="A534" s="5">
+      <c r="A534" s="7">
         <v>43585.904541890952</v>
       </c>
       <c r="B534">
@@ -4654,7 +4658,7 @@
       </c>
     </row>
     <row r="535">
-      <c r="A535" s="5">
+      <c r="A535" s="7">
         <v>43585.904555625748</v>
       </c>
       <c r="B535">
@@ -4662,7 +4666,7 @@
       </c>
     </row>
     <row r="536">
-      <c r="A536" s="5">
+      <c r="A536" s="7">
         <v>43585.904569538659</v>
       </c>
       <c r="B536">
@@ -4670,7 +4674,7 @@
       </c>
     </row>
     <row r="537">
-      <c r="A537" s="5">
+      <c r="A537" s="7">
         <v>43585.904583406751</v>
       </c>
       <c r="B537">
@@ -4678,7 +4682,7 @@
       </c>
     </row>
     <row r="538">
-      <c r="A538" s="5">
+      <c r="A538" s="7">
         <v>43585.904596924083</v>
       </c>
       <c r="B538">
@@ -4686,7 +4690,7 @@
       </c>
     </row>
     <row r="539">
-      <c r="A539" s="5">
+      <c r="A539" s="7">
         <v>43585.90468211448</v>
       </c>
       <c r="B539">
@@ -4694,7 +4698,7 @@
       </c>
     </row>
     <row r="540">
-      <c r="A540" s="5">
+      <c r="A540" s="7">
         <v>43585.904690257506</v>
       </c>
       <c r="B540">
@@ -4702,7 +4706,7 @@
       </c>
     </row>
     <row r="541">
-      <c r="A541" s="5">
+      <c r="A541" s="7">
         <v>43585.904698564445</v>
       </c>
       <c r="B541">
@@ -4710,7 +4714,7 @@
       </c>
     </row>
     <row r="542">
-      <c r="A542" s="5">
+      <c r="A542" s="7">
         <v>43585.904707132257</v>
       </c>
       <c r="B542">
@@ -4718,7 +4722,7 @@
       </c>
     </row>
     <row r="543">
-      <c r="A543" s="5">
+      <c r="A543" s="7">
         <v>43585.904716014047</v>
       </c>
       <c r="B543">
@@ -4726,7 +4730,7 @@
       </c>
     </row>
     <row r="544">
-      <c r="A544" s="5">
+      <c r="A544" s="7">
         <v>43585.904724703752</v>
       </c>
       <c r="B544">
@@ -4734,7 +4738,7 @@
       </c>
     </row>
     <row r="545">
-      <c r="A545" s="5">
+      <c r="A545" s="7">
         <v>43585.904733632808</v>
       </c>
       <c r="B545">
@@ -4742,7 +4746,7 @@
       </c>
     </row>
     <row r="546">
-      <c r="A546" s="5">
+      <c r="A546" s="7">
         <v>43585.904742543469</v>
       </c>
       <c r="B546">
@@ -4750,7 +4754,7 @@
       </c>
     </row>
     <row r="547">
-      <c r="A547" s="5">
+      <c r="A547" s="7">
         <v>43585.904751443653</v>
       </c>
       <c r="B547">
@@ -4758,7 +4762,7 @@
       </c>
     </row>
     <row r="548">
-      <c r="A548" s="5">
+      <c r="A548" s="7">
         <v>43585.904760410427</v>
       </c>
       <c r="B548">
@@ -4766,7 +4770,7 @@
       </c>
     </row>
     <row r="549">
-      <c r="A549" s="5">
+      <c r="A549" s="7">
         <v>43585.904769096989</v>
       </c>
       <c r="B549">
@@ -4774,7 +4778,7 @@
       </c>
     </row>
     <row r="550">
-      <c r="A550" s="5">
+      <c r="A550" s="7">
         <v>43585.904777938034</v>
       </c>
       <c r="B550">

</xml_diff>